<commit_message>
[UPDATE] - Montly Report MK Snack & Spesial
</commit_message>
<xml_diff>
--- a/resources/template/WASTU.xlsx
+++ b/resources/template/WASTU.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hallo_ppa\resources\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D69E259-184F-4EC4-872B-9C20CEFD5BA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32474D05-02CA-4984-8B78-769DC5B8002C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{96DAB095-C63E-43E2-9BFC-56E2EB8E01C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="111">
   <si>
     <t>Prod PIT 2</t>
   </si>
@@ -354,13 +354,22 @@
   </si>
   <si>
     <t>Dept.Head FALOG ★(WAREHOUSE)</t>
+  </si>
+  <si>
+    <t>MK SPESIAL</t>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>MK SNACK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -421,8 +430,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -513,8 +530,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -631,11 +660,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -764,6 +813,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -771,9 +823,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -791,19 +840,7 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -818,8 +855,42 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1145,15 +1216,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{727E0051-6F26-4AB8-8E1A-F7C7AFECA816}">
-  <dimension ref="A1:AK113"/>
+  <dimension ref="A1:AK151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J80" sqref="J80"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="A115" sqref="A115:AJ115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="32.33203125" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="71"/>
+    <col min="3" max="3" width="32.33203125" style="71" customWidth="1"/>
     <col min="4" max="4" width="44.109375" customWidth="1"/>
     <col min="5" max="5" width="9" style="45" customWidth="1"/>
     <col min="6" max="35" width="8.88671875" style="45"/>
@@ -1442,7 +1514,7 @@
     <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A6" s="53"/>
       <c r="B6" s="51"/>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="47" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="6" t="s">
@@ -1487,7 +1559,7 @@
     <row r="7" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A7" s="53"/>
       <c r="B7" s="51"/>
-      <c r="C7" s="46"/>
+      <c r="C7" s="47"/>
       <c r="D7" s="6" t="s">
         <v>12</v>
       </c>
@@ -1530,7 +1602,7 @@
     <row r="8" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A8" s="53"/>
       <c r="B8" s="51"/>
-      <c r="C8" s="46"/>
+      <c r="C8" s="47"/>
       <c r="D8" s="6" t="s">
         <v>13</v>
       </c>
@@ -1618,7 +1690,7 @@
     <row r="10" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A10" s="53"/>
       <c r="B10" s="51"/>
-      <c r="C10" s="47" t="s">
+      <c r="C10" s="48" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="11" t="s">
@@ -1663,7 +1735,7 @@
     <row r="11" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A11" s="53"/>
       <c r="B11" s="51"/>
-      <c r="C11" s="47"/>
+      <c r="C11" s="48"/>
       <c r="D11" s="11" t="s">
         <v>18</v>
       </c>
@@ -1706,7 +1778,7 @@
     <row r="12" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A12" s="53"/>
       <c r="B12" s="51"/>
-      <c r="C12" s="47"/>
+      <c r="C12" s="48"/>
       <c r="D12" s="11" t="s">
         <v>19</v>
       </c>
@@ -1749,7 +1821,7 @@
     <row r="13" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A13" s="53"/>
       <c r="B13" s="51"/>
-      <c r="C13" s="47"/>
+      <c r="C13" s="48"/>
       <c r="D13" s="11" t="s">
         <v>20</v>
       </c>
@@ -1792,7 +1864,7 @@
     <row r="14" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A14" s="53"/>
       <c r="B14" s="51"/>
-      <c r="C14" s="47" t="s">
+      <c r="C14" s="48" t="s">
         <v>21</v>
       </c>
       <c r="D14" s="11" t="s">
@@ -1837,7 +1909,7 @@
     <row r="15" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A15" s="53"/>
       <c r="B15" s="51"/>
-      <c r="C15" s="47"/>
+      <c r="C15" s="48"/>
       <c r="D15" s="11" t="s">
         <v>23</v>
       </c>
@@ -1880,7 +1952,7 @@
     <row r="16" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A16" s="53"/>
       <c r="B16" s="51"/>
-      <c r="C16" s="47"/>
+      <c r="C16" s="48"/>
       <c r="D16" s="11" t="s">
         <v>24</v>
       </c>
@@ -1923,7 +1995,7 @@
     <row r="17" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A17" s="53"/>
       <c r="B17" s="51"/>
-      <c r="C17" s="47"/>
+      <c r="C17" s="48"/>
       <c r="D17" s="11" t="s">
         <v>25</v>
       </c>
@@ -1966,7 +2038,7 @@
     <row r="18" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A18" s="53"/>
       <c r="B18" s="51"/>
-      <c r="C18" s="47"/>
+      <c r="C18" s="48"/>
       <c r="D18" s="11" t="s">
         <v>26</v>
       </c>
@@ -2009,7 +2081,7 @@
     <row r="19" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A19" s="53"/>
       <c r="B19" s="51"/>
-      <c r="C19" s="47"/>
+      <c r="C19" s="48"/>
       <c r="D19" s="11" t="s">
         <v>27</v>
       </c>
@@ -2052,7 +2124,7 @@
     <row r="20" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A20" s="53"/>
       <c r="B20" s="51"/>
-      <c r="C20" s="60" t="s">
+      <c r="C20" s="56" t="s">
         <v>28</v>
       </c>
       <c r="D20" s="8" t="s">
@@ -2097,7 +2169,7 @@
     <row r="21" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A21" s="53"/>
       <c r="B21" s="51"/>
-      <c r="C21" s="60"/>
+      <c r="C21" s="56"/>
       <c r="D21" s="20" t="s">
         <v>102</v>
       </c>
@@ -2137,7 +2209,7 @@
     <row r="22" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A22" s="53"/>
       <c r="B22" s="51"/>
-      <c r="C22" s="60"/>
+      <c r="C22" s="56"/>
       <c r="D22" s="8" t="s">
         <v>30</v>
       </c>
@@ -2180,7 +2252,7 @@
     <row r="23" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A23" s="53"/>
       <c r="B23" s="51"/>
-      <c r="C23" s="60"/>
+      <c r="C23" s="56"/>
       <c r="D23" s="8" t="s">
         <v>31</v>
       </c>
@@ -2223,7 +2295,7 @@
     <row r="24" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A24" s="53"/>
       <c r="B24" s="51"/>
-      <c r="C24" s="60"/>
+      <c r="C24" s="56"/>
       <c r="D24" s="8" t="s">
         <v>32</v>
       </c>
@@ -2266,7 +2338,7 @@
     <row r="25" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A25" s="53"/>
       <c r="B25" s="51"/>
-      <c r="C25" s="60"/>
+      <c r="C25" s="56"/>
       <c r="D25" s="8" t="s">
         <v>33</v>
       </c>
@@ -2309,7 +2381,7 @@
     <row r="26" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A26" s="53"/>
       <c r="B26" s="51"/>
-      <c r="C26" s="60"/>
+      <c r="C26" s="56"/>
       <c r="D26" s="8" t="s">
         <v>34</v>
       </c>
@@ -2352,7 +2424,7 @@
     <row r="27" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A27" s="53"/>
       <c r="B27" s="51"/>
-      <c r="C27" s="60"/>
+      <c r="C27" s="56"/>
       <c r="D27" s="8" t="s">
         <v>35</v>
       </c>
@@ -2395,7 +2467,7 @@
     <row r="28" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A28" s="53"/>
       <c r="B28" s="51"/>
-      <c r="C28" s="60"/>
+      <c r="C28" s="56"/>
       <c r="D28" s="8" t="s">
         <v>36</v>
       </c>
@@ -2438,7 +2510,7 @@
     <row r="29" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A29" s="53"/>
       <c r="B29" s="51"/>
-      <c r="C29" s="60"/>
+      <c r="C29" s="56"/>
       <c r="D29" s="8" t="s">
         <v>37</v>
       </c>
@@ -2481,7 +2553,7 @@
     <row r="30" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A30" s="53"/>
       <c r="B30" s="51"/>
-      <c r="C30" s="61" t="s">
+      <c r="C30" s="57" t="s">
         <v>38</v>
       </c>
       <c r="D30" s="9" t="s">
@@ -2526,7 +2598,7 @@
     <row r="31" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A31" s="53"/>
       <c r="B31" s="51"/>
-      <c r="C31" s="61"/>
+      <c r="C31" s="57"/>
       <c r="D31" s="9" t="s">
         <v>31</v>
       </c>
@@ -2569,7 +2641,7 @@
     <row r="32" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A32" s="53"/>
       <c r="B32" s="51"/>
-      <c r="C32" s="61"/>
+      <c r="C32" s="57"/>
       <c r="D32" s="9" t="s">
         <v>32</v>
       </c>
@@ -2612,7 +2684,7 @@
     <row r="33" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A33" s="53"/>
       <c r="B33" s="51"/>
-      <c r="C33" s="61"/>
+      <c r="C33" s="57"/>
       <c r="D33" s="9" t="s">
         <v>33</v>
       </c>
@@ -2655,7 +2727,7 @@
     <row r="34" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A34" s="53"/>
       <c r="B34" s="51"/>
-      <c r="C34" s="61"/>
+      <c r="C34" s="57"/>
       <c r="D34" s="9" t="s">
         <v>34</v>
       </c>
@@ -2698,7 +2770,7 @@
     <row r="35" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A35" s="53"/>
       <c r="B35" s="51"/>
-      <c r="C35" s="61"/>
+      <c r="C35" s="57"/>
       <c r="D35" s="9" t="s">
         <v>35</v>
       </c>
@@ -2741,7 +2813,7 @@
     <row r="36" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A36" s="53"/>
       <c r="B36" s="51"/>
-      <c r="C36" s="61"/>
+      <c r="C36" s="57"/>
       <c r="D36" s="9" t="s">
         <v>36</v>
       </c>
@@ -2784,7 +2856,7 @@
     <row r="37" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A37" s="53"/>
       <c r="B37" s="51"/>
-      <c r="C37" s="61"/>
+      <c r="C37" s="57"/>
       <c r="D37" s="9" t="s">
         <v>37</v>
       </c>
@@ -2827,7 +2899,7 @@
     <row r="38" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A38" s="53"/>
       <c r="B38" s="51"/>
-      <c r="C38" s="61"/>
+      <c r="C38" s="57"/>
       <c r="D38" s="9" t="s">
         <v>39</v>
       </c>
@@ -2870,7 +2942,7 @@
     <row r="39" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A39" s="53"/>
       <c r="B39" s="51"/>
-      <c r="C39" s="62" t="s">
+      <c r="C39" s="58" t="s">
         <v>40</v>
       </c>
       <c r="D39" s="19" t="s">
@@ -2915,7 +2987,7 @@
     <row r="40" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A40" s="53"/>
       <c r="B40" s="51"/>
-      <c r="C40" s="62"/>
+      <c r="C40" s="58"/>
       <c r="D40" s="19" t="s">
         <v>42</v>
       </c>
@@ -2958,7 +3030,7 @@
     <row r="41" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A41" s="53"/>
       <c r="B41" s="51"/>
-      <c r="C41" s="62"/>
+      <c r="C41" s="58"/>
       <c r="D41" s="19" t="s">
         <v>43</v>
       </c>
@@ -3001,7 +3073,7 @@
     <row r="42" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A42" s="53"/>
       <c r="B42" s="51"/>
-      <c r="C42" s="62"/>
+      <c r="C42" s="58"/>
       <c r="D42" s="19" t="s">
         <v>44</v>
       </c>
@@ -3044,7 +3116,7 @@
     <row r="43" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A43" s="53"/>
       <c r="B43" s="51"/>
-      <c r="C43" s="62"/>
+      <c r="C43" s="58"/>
       <c r="D43" s="19" t="s">
         <v>45</v>
       </c>
@@ -3087,7 +3159,7 @@
     <row r="44" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A44" s="53"/>
       <c r="B44" s="51"/>
-      <c r="C44" s="62"/>
+      <c r="C44" s="58"/>
       <c r="D44" s="19" t="s">
         <v>46</v>
       </c>
@@ -3130,7 +3202,7 @@
     <row r="45" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A45" s="53"/>
       <c r="B45" s="51"/>
-      <c r="C45" s="62"/>
+      <c r="C45" s="58"/>
       <c r="D45" s="19" t="s">
         <v>47</v>
       </c>
@@ -3173,7 +3245,7 @@
     <row r="46" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A46" s="53"/>
       <c r="B46" s="51"/>
-      <c r="C46" s="62"/>
+      <c r="C46" s="58"/>
       <c r="D46" s="19" t="s">
         <v>48</v>
       </c>
@@ -3216,7 +3288,7 @@
     <row r="47" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A47" s="53"/>
       <c r="B47" s="51"/>
-      <c r="C47" s="62"/>
+      <c r="C47" s="58"/>
       <c r="D47" s="19" t="s">
         <v>49</v>
       </c>
@@ -3259,7 +3331,7 @@
     <row r="48" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A48" s="53"/>
       <c r="B48" s="51"/>
-      <c r="C48" s="62"/>
+      <c r="C48" s="58"/>
       <c r="D48" s="19" t="s">
         <v>50</v>
       </c>
@@ -3302,7 +3374,7 @@
     <row r="49" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A49" s="53"/>
       <c r="B49" s="51"/>
-      <c r="C49" s="62"/>
+      <c r="C49" s="58"/>
       <c r="D49" s="19" t="s">
         <v>51</v>
       </c>
@@ -3345,7 +3417,7 @@
     <row r="50" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A50" s="53"/>
       <c r="B50" s="51"/>
-      <c r="C50" s="63" t="s">
+      <c r="C50" s="59" t="s">
         <v>52</v>
       </c>
       <c r="D50" s="18" t="s">
@@ -3390,7 +3462,7 @@
     <row r="51" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A51" s="53"/>
       <c r="B51" s="51"/>
-      <c r="C51" s="63"/>
+      <c r="C51" s="59"/>
       <c r="D51" s="18" t="s">
         <v>54</v>
       </c>
@@ -3433,7 +3505,7 @@
     <row r="52" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A52" s="53"/>
       <c r="B52" s="51"/>
-      <c r="C52" s="63"/>
+      <c r="C52" s="59"/>
       <c r="D52" s="18" t="s">
         <v>55</v>
       </c>
@@ -3476,7 +3548,7 @@
     <row r="53" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A53" s="53"/>
       <c r="B53" s="51"/>
-      <c r="C53" s="63"/>
+      <c r="C53" s="59"/>
       <c r="D53" s="18" t="s">
         <v>56</v>
       </c>
@@ -3519,7 +3591,7 @@
     <row r="54" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A54" s="53"/>
       <c r="B54" s="51"/>
-      <c r="C54" s="63"/>
+      <c r="C54" s="59"/>
       <c r="D54" s="18" t="s">
         <v>57</v>
       </c>
@@ -3562,7 +3634,7 @@
     <row r="55" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A55" s="53"/>
       <c r="B55" s="51"/>
-      <c r="C55" s="63"/>
+      <c r="C55" s="59"/>
       <c r="D55" s="18" t="s">
         <v>58</v>
       </c>
@@ -3605,7 +3677,7 @@
     <row r="56" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A56" s="53"/>
       <c r="B56" s="51"/>
-      <c r="C56" s="63"/>
+      <c r="C56" s="59"/>
       <c r="D56" s="40" t="s">
         <v>59</v>
       </c>
@@ -3645,7 +3717,7 @@
     <row r="57" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A57" s="53"/>
       <c r="B57" s="51"/>
-      <c r="C57" s="63"/>
+      <c r="C57" s="59"/>
       <c r="D57" s="41" t="s">
         <v>107</v>
       </c>
@@ -3773,7 +3845,7 @@
     <row r="60" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A60" s="53"/>
       <c r="B60" s="51"/>
-      <c r="C60" s="55"/>
+      <c r="C60" s="67"/>
       <c r="D60" s="13" t="s">
         <v>62</v>
       </c>
@@ -3816,7 +3888,7 @@
     <row r="61" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A61" s="53"/>
       <c r="B61" s="51"/>
-      <c r="C61" s="55"/>
+      <c r="C61" s="67"/>
       <c r="D61" s="13" t="s">
         <v>63</v>
       </c>
@@ -3859,7 +3931,7 @@
     <row r="62" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A62" s="53"/>
       <c r="B62" s="51"/>
-      <c r="C62" s="55"/>
+      <c r="C62" s="67"/>
       <c r="D62" s="13" t="s">
         <v>64</v>
       </c>
@@ -3902,7 +3974,7 @@
     <row r="63" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A63" s="53"/>
       <c r="B63" s="51"/>
-      <c r="C63" s="55"/>
+      <c r="C63" s="67"/>
       <c r="D63" s="13" t="s">
         <v>65</v>
       </c>
@@ -3945,7 +4017,7 @@
     <row r="64" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A64" s="53"/>
       <c r="B64" s="51"/>
-      <c r="C64" s="55"/>
+      <c r="C64" s="67"/>
       <c r="D64" s="13" t="s">
         <v>66</v>
       </c>
@@ -3988,7 +4060,7 @@
     <row r="65" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A65" s="53"/>
       <c r="B65" s="51"/>
-      <c r="C65" s="55"/>
+      <c r="C65" s="67"/>
       <c r="D65" s="13" t="s">
         <v>67</v>
       </c>
@@ -4031,7 +4103,7 @@
     <row r="66" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A66" s="53"/>
       <c r="B66" s="51"/>
-      <c r="C66" s="55"/>
+      <c r="C66" s="67"/>
       <c r="D66" s="13" t="s">
         <v>68</v>
       </c>
@@ -4074,7 +4146,7 @@
     <row r="67" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A67" s="53"/>
       <c r="B67" s="51"/>
-      <c r="C67" s="55"/>
+      <c r="C67" s="67"/>
       <c r="D67" s="13" t="s">
         <v>69</v>
       </c>
@@ -4117,7 +4189,7 @@
     <row r="68" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A68" s="53"/>
       <c r="B68" s="51"/>
-      <c r="C68" s="55"/>
+      <c r="C68" s="67"/>
       <c r="D68" s="13" t="s">
         <v>70</v>
       </c>
@@ -4160,7 +4232,7 @@
     <row r="69" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A69" s="53"/>
       <c r="B69" s="51"/>
-      <c r="C69" s="55"/>
+      <c r="C69" s="67"/>
       <c r="D69" s="13" t="s">
         <v>71</v>
       </c>
@@ -4203,7 +4275,7 @@
     <row r="70" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A70" s="53"/>
       <c r="B70" s="51"/>
-      <c r="C70" s="55"/>
+      <c r="C70" s="67"/>
       <c r="D70" s="13" t="s">
         <v>72</v>
       </c>
@@ -4246,7 +4318,7 @@
     <row r="71" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A71" s="53"/>
       <c r="B71" s="51"/>
-      <c r="C71" s="55"/>
+      <c r="C71" s="67"/>
       <c r="D71" s="13" t="s">
         <v>73</v>
       </c>
@@ -4289,7 +4361,7 @@
     <row r="72" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A72" s="53"/>
       <c r="B72" s="51"/>
-      <c r="C72" s="56"/>
+      <c r="C72" s="68"/>
       <c r="D72" s="13" t="s">
         <v>74</v>
       </c>
@@ -4417,7 +4489,7 @@
     <row r="75" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="53"/>
       <c r="B75" s="51"/>
-      <c r="C75" s="57" t="s">
+      <c r="C75" s="55" t="s">
         <v>75</v>
       </c>
       <c r="D75" s="15" t="s">
@@ -4462,7 +4534,7 @@
     <row r="76" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="53"/>
       <c r="B76" s="51"/>
-      <c r="C76" s="58"/>
+      <c r="C76" s="69"/>
       <c r="D76" s="15" t="s">
         <v>77</v>
       </c>
@@ -4505,7 +4577,7 @@
     <row r="77" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" s="53"/>
       <c r="B77" s="51"/>
-      <c r="C77" s="58"/>
+      <c r="C77" s="69"/>
       <c r="D77" s="15" t="s">
         <v>78</v>
       </c>
@@ -4548,7 +4620,7 @@
     <row r="78" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="53"/>
       <c r="B78" s="51"/>
-      <c r="C78" s="58"/>
+      <c r="C78" s="69"/>
       <c r="D78" s="15" t="s">
         <v>79</v>
       </c>
@@ -4591,7 +4663,7 @@
     <row r="79" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A79" s="53"/>
       <c r="B79" s="51"/>
-      <c r="C79" s="58"/>
+      <c r="C79" s="69"/>
       <c r="D79" s="15" t="s">
         <v>80</v>
       </c>
@@ -4634,7 +4706,7 @@
     <row r="80" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A80" s="53"/>
       <c r="B80" s="51"/>
-      <c r="C80" s="58"/>
+      <c r="C80" s="69"/>
       <c r="D80" s="16" t="s">
         <v>81</v>
       </c>
@@ -4677,7 +4749,7 @@
     <row r="81" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" s="53"/>
       <c r="B81" s="51"/>
-      <c r="C81" s="58"/>
+      <c r="C81" s="69"/>
       <c r="D81" s="15" t="s">
         <v>82</v>
       </c>
@@ -4720,7 +4792,7 @@
     <row r="82" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="53"/>
       <c r="B82" s="51"/>
-      <c r="C82" s="58"/>
+      <c r="C82" s="69"/>
       <c r="D82" s="15" t="s">
         <v>83</v>
       </c>
@@ -4763,7 +4835,7 @@
     <row r="83" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A83" s="53"/>
       <c r="B83" s="51"/>
-      <c r="C83" s="58"/>
+      <c r="C83" s="69"/>
       <c r="D83" s="15" t="s">
         <v>41</v>
       </c>
@@ -4806,7 +4878,7 @@
     <row r="84" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A84" s="53"/>
       <c r="B84" s="51"/>
-      <c r="C84" s="58"/>
+      <c r="C84" s="69"/>
       <c r="D84" s="15" t="s">
         <v>84</v>
       </c>
@@ -4849,7 +4921,7 @@
     <row r="85" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="53"/>
       <c r="B85" s="51"/>
-      <c r="C85" s="58"/>
+      <c r="C85" s="69"/>
       <c r="D85" s="15" t="s">
         <v>85</v>
       </c>
@@ -4892,7 +4964,7 @@
     <row r="86" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" s="53"/>
       <c r="B86" s="51"/>
-      <c r="C86" s="58"/>
+      <c r="C86" s="69"/>
       <c r="D86" s="15" t="s">
         <v>48</v>
       </c>
@@ -4935,7 +5007,7 @@
     <row r="87" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="53"/>
       <c r="B87" s="51"/>
-      <c r="C87" s="58"/>
+      <c r="C87" s="69"/>
       <c r="D87" s="15" t="s">
         <v>86</v>
       </c>
@@ -4978,7 +5050,7 @@
     <row r="88" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" s="53"/>
       <c r="B88" s="51"/>
-      <c r="C88" s="58"/>
+      <c r="C88" s="69"/>
       <c r="D88" s="15" t="s">
         <v>87</v>
       </c>
@@ -5021,7 +5093,7 @@
     <row r="89" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A89" s="53"/>
       <c r="B89" s="51"/>
-      <c r="C89" s="58"/>
+      <c r="C89" s="69"/>
       <c r="D89" s="15" t="s">
         <v>88</v>
       </c>
@@ -5064,7 +5136,7 @@
     <row r="90" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" s="53"/>
       <c r="B90" s="51"/>
-      <c r="C90" s="58"/>
+      <c r="C90" s="69"/>
       <c r="D90" s="15" t="s">
         <v>2</v>
       </c>
@@ -5107,7 +5179,7 @@
     <row r="91" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" s="53"/>
       <c r="B91" s="51"/>
-      <c r="C91" s="58"/>
+      <c r="C91" s="69"/>
       <c r="D91" s="15" t="s">
         <v>0</v>
       </c>
@@ -5150,7 +5222,7 @@
     <row r="92" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A92" s="53"/>
       <c r="B92" s="51"/>
-      <c r="C92" s="58"/>
+      <c r="C92" s="69"/>
       <c r="D92" s="15" t="s">
         <v>1</v>
       </c>
@@ -5193,7 +5265,7 @@
     <row r="93" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A93" s="53"/>
       <c r="B93" s="51"/>
-      <c r="C93" s="58"/>
+      <c r="C93" s="69"/>
       <c r="D93" s="15" t="s">
         <v>89</v>
       </c>
@@ -5236,7 +5308,7 @@
     <row r="94" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A94" s="53"/>
       <c r="B94" s="51"/>
-      <c r="C94" s="58"/>
+      <c r="C94" s="69"/>
       <c r="D94" s="15" t="s">
         <v>90</v>
       </c>
@@ -5279,7 +5351,7 @@
     <row r="95" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A95" s="53"/>
       <c r="B95" s="51"/>
-      <c r="C95" s="58"/>
+      <c r="C95" s="69"/>
       <c r="D95" s="15" t="s">
         <v>91</v>
       </c>
@@ -5322,7 +5394,7 @@
     <row r="96" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A96" s="53"/>
       <c r="B96" s="51"/>
-      <c r="C96" s="58"/>
+      <c r="C96" s="69"/>
       <c r="D96" s="15" t="s">
         <v>92</v>
       </c>
@@ -5365,7 +5437,7 @@
     <row r="97" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A97" s="53"/>
       <c r="B97" s="51"/>
-      <c r="C97" s="58"/>
+      <c r="C97" s="69"/>
       <c r="D97" s="15" t="s">
         <v>93</v>
       </c>
@@ -5408,7 +5480,7 @@
     <row r="98" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A98" s="53"/>
       <c r="B98" s="51"/>
-      <c r="C98" s="58"/>
+      <c r="C98" s="69"/>
       <c r="D98" s="15" t="s">
         <v>94</v>
       </c>
@@ -5451,7 +5523,7 @@
     <row r="99" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A99" s="53"/>
       <c r="B99" s="51"/>
-      <c r="C99" s="58"/>
+      <c r="C99" s="69"/>
       <c r="D99" s="15" t="s">
         <v>95</v>
       </c>
@@ -5494,7 +5566,7 @@
     <row r="100" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A100" s="53"/>
       <c r="B100" s="51"/>
-      <c r="C100" s="58"/>
+      <c r="C100" s="69"/>
       <c r="D100" s="15" t="s">
         <v>96</v>
       </c>
@@ -5537,7 +5609,7 @@
     <row r="101" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A101" s="53"/>
       <c r="B101" s="51"/>
-      <c r="C101" s="58"/>
+      <c r="C101" s="69"/>
       <c r="D101" s="15" t="s">
         <v>97</v>
       </c>
@@ -5580,7 +5652,7 @@
     <row r="102" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A102" s="53"/>
       <c r="B102" s="51"/>
-      <c r="C102" s="58"/>
+      <c r="C102" s="69"/>
       <c r="D102" s="15" t="s">
         <v>98</v>
       </c>
@@ -5623,7 +5695,7 @@
     <row r="103" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A103" s="53"/>
       <c r="B103" s="51"/>
-      <c r="C103" s="58"/>
+      <c r="C103" s="69"/>
       <c r="D103" s="15" t="s">
         <v>99</v>
       </c>
@@ -5666,7 +5738,7 @@
     <row r="104" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A104" s="53"/>
       <c r="B104" s="51"/>
-      <c r="C104" s="59"/>
+      <c r="C104" s="70"/>
       <c r="D104" s="15" t="s">
         <v>100</v>
       </c>
@@ -5749,7 +5821,7 @@
     <row r="106" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A106" s="53"/>
       <c r="B106" s="51"/>
-      <c r="C106" s="48" t="s">
+      <c r="C106" s="49" t="s">
         <v>106</v>
       </c>
       <c r="D106" s="28" t="s">
@@ -5964,132 +6036,132 @@
       </c>
     </row>
     <row r="111" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="E111" s="64">
+      <c r="E111" s="46">
         <f>SUM(E3:E110)</f>
         <v>0</v>
       </c>
-      <c r="F111" s="64">
+      <c r="F111" s="46">
         <f>SUM(F3:F110)</f>
         <v>0</v>
       </c>
-      <c r="G111" s="64">
+      <c r="G111" s="46">
         <f t="shared" ref="G111:AI111" si="2">SUM(G3:G110)</f>
         <v>0</v>
       </c>
-      <c r="H111" s="64">
+      <c r="H111" s="46">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I111" s="64">
+      <c r="I111" s="46">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J111" s="64">
+      <c r="J111" s="46">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K111" s="64">
+      <c r="K111" s="46">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L111" s="64">
+      <c r="L111" s="46">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M111" s="64">
+      <c r="M111" s="46">
         <f>SUM(M3:M110)</f>
         <v>0</v>
       </c>
-      <c r="N111" s="64">
+      <c r="N111" s="46">
         <f>SUM(N3:N110)</f>
         <v>0</v>
       </c>
-      <c r="O111" s="64">
+      <c r="O111" s="46">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P111" s="64">
+      <c r="P111" s="46">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q111" s="64">
+      <c r="Q111" s="46">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R111" s="64">
+      <c r="R111" s="46">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S111" s="64">
+      <c r="S111" s="46">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T111" s="64">
+      <c r="T111" s="46">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U111" s="64">
+      <c r="U111" s="46">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="V111" s="64">
+      <c r="V111" s="46">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="W111" s="64">
+      <c r="W111" s="46">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X111" s="64">
+      <c r="X111" s="46">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y111" s="64">
+      <c r="Y111" s="46">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Z111" s="64">
+      <c r="Z111" s="46">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA111" s="64">
+      <c r="AA111" s="46">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB111" s="64">
+      <c r="AB111" s="46">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC111" s="64">
+      <c r="AC111" s="46">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AD111" s="64">
+      <c r="AD111" s="46">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AE111" s="64">
+      <c r="AE111" s="46">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AF111" s="64">
+      <c r="AF111" s="46">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AG111" s="64">
+      <c r="AG111" s="46">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AH111" s="64">
+      <c r="AH111" s="46">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AI111" s="64">
+      <c r="AI111" s="46">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="35:36" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:36" x14ac:dyDescent="0.3">
       <c r="AI113" s="26" t="s">
         <v>5</v>
       </c>
@@ -6098,8 +6170,1528 @@
         <v>0</v>
       </c>
     </row>
+    <row r="115" spans="1:36" ht="18" x14ac:dyDescent="0.3">
+      <c r="A115" s="60" t="s">
+        <v>108</v>
+      </c>
+      <c r="B115" s="61"/>
+      <c r="C115" s="61"/>
+      <c r="D115" s="61"/>
+      <c r="E115" s="61"/>
+      <c r="F115" s="61"/>
+      <c r="G115" s="61"/>
+      <c r="H115" s="61"/>
+      <c r="I115" s="61"/>
+      <c r="J115" s="61"/>
+      <c r="K115" s="61"/>
+      <c r="L115" s="61"/>
+      <c r="M115" s="61"/>
+      <c r="N115" s="61"/>
+      <c r="O115" s="61"/>
+      <c r="P115" s="61"/>
+      <c r="Q115" s="61"/>
+      <c r="R115" s="61"/>
+      <c r="S115" s="61"/>
+      <c r="T115" s="61"/>
+      <c r="U115" s="61"/>
+      <c r="V115" s="61"/>
+      <c r="W115" s="61"/>
+      <c r="X115" s="61"/>
+      <c r="Y115" s="61"/>
+      <c r="Z115" s="61"/>
+      <c r="AA115" s="61"/>
+      <c r="AB115" s="61"/>
+      <c r="AC115" s="61"/>
+      <c r="AD115" s="61"/>
+      <c r="AE115" s="61"/>
+      <c r="AF115" s="61"/>
+      <c r="AG115" s="61"/>
+      <c r="AH115" s="61"/>
+      <c r="AI115" s="61"/>
+      <c r="AJ115" s="61"/>
+    </row>
+    <row r="116" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A116" s="72"/>
+      <c r="B116" s="62" t="s">
+        <v>109</v>
+      </c>
+      <c r="C116" s="63" t="s">
+        <v>4</v>
+      </c>
+      <c r="D116" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="E116" s="64">
+        <v>1</v>
+      </c>
+      <c r="F116" s="64">
+        <v>2</v>
+      </c>
+      <c r="G116" s="64">
+        <v>3</v>
+      </c>
+      <c r="H116" s="64">
+        <v>4</v>
+      </c>
+      <c r="I116" s="64">
+        <v>5</v>
+      </c>
+      <c r="J116" s="64">
+        <v>6</v>
+      </c>
+      <c r="K116" s="64">
+        <v>7</v>
+      </c>
+      <c r="L116" s="64">
+        <v>8</v>
+      </c>
+      <c r="M116" s="64">
+        <v>9</v>
+      </c>
+      <c r="N116" s="64">
+        <v>10</v>
+      </c>
+      <c r="O116" s="64">
+        <v>11</v>
+      </c>
+      <c r="P116" s="64">
+        <v>12</v>
+      </c>
+      <c r="Q116" s="64">
+        <v>13</v>
+      </c>
+      <c r="R116" s="64">
+        <v>14</v>
+      </c>
+      <c r="S116" s="64">
+        <v>15</v>
+      </c>
+      <c r="T116" s="64">
+        <v>16</v>
+      </c>
+      <c r="U116" s="64">
+        <v>17</v>
+      </c>
+      <c r="V116" s="64">
+        <v>18</v>
+      </c>
+      <c r="W116" s="64">
+        <v>19</v>
+      </c>
+      <c r="X116" s="64">
+        <v>20</v>
+      </c>
+      <c r="Y116" s="64">
+        <v>21</v>
+      </c>
+      <c r="Z116" s="64">
+        <v>22</v>
+      </c>
+      <c r="AA116" s="64">
+        <v>23</v>
+      </c>
+      <c r="AB116" s="64">
+        <v>24</v>
+      </c>
+      <c r="AC116" s="64">
+        <v>25</v>
+      </c>
+      <c r="AD116" s="64">
+        <v>26</v>
+      </c>
+      <c r="AE116" s="64">
+        <v>27</v>
+      </c>
+      <c r="AF116" s="64">
+        <v>28</v>
+      </c>
+      <c r="AG116" s="64">
+        <v>29</v>
+      </c>
+      <c r="AH116" s="64">
+        <v>30</v>
+      </c>
+      <c r="AI116" s="64">
+        <v>31</v>
+      </c>
+      <c r="AJ116" s="65" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A117" s="25"/>
+      <c r="B117" s="66"/>
+      <c r="C117" s="66"/>
+      <c r="D117" s="25"/>
+      <c r="E117" s="25"/>
+      <c r="F117" s="25"/>
+      <c r="G117" s="25"/>
+      <c r="H117" s="25"/>
+      <c r="I117" s="25"/>
+      <c r="J117" s="25"/>
+      <c r="K117" s="25"/>
+      <c r="L117" s="25"/>
+      <c r="M117" s="25"/>
+      <c r="N117" s="25"/>
+      <c r="O117" s="25"/>
+      <c r="P117" s="25"/>
+      <c r="Q117" s="25"/>
+      <c r="R117" s="25"/>
+      <c r="S117" s="25"/>
+      <c r="T117" s="25"/>
+      <c r="U117" s="25"/>
+      <c r="V117" s="25"/>
+      <c r="W117" s="25"/>
+      <c r="X117" s="25"/>
+      <c r="Y117" s="25"/>
+      <c r="Z117" s="25"/>
+      <c r="AA117" s="25"/>
+      <c r="AB117" s="25"/>
+      <c r="AC117" s="25"/>
+      <c r="AD117" s="25"/>
+      <c r="AE117" s="25"/>
+      <c r="AF117" s="25"/>
+      <c r="AG117" s="25"/>
+      <c r="AH117" s="25"/>
+      <c r="AI117" s="25"/>
+    </row>
+    <row r="118" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A118" s="25"/>
+      <c r="B118" s="66"/>
+      <c r="C118" s="66"/>
+      <c r="D118" s="25"/>
+      <c r="E118" s="25"/>
+      <c r="F118" s="25"/>
+      <c r="G118" s="25"/>
+      <c r="H118" s="25"/>
+      <c r="I118" s="25"/>
+      <c r="J118" s="25"/>
+      <c r="K118" s="25"/>
+      <c r="L118" s="25"/>
+      <c r="M118" s="25"/>
+      <c r="N118" s="25"/>
+      <c r="O118" s="25"/>
+      <c r="P118" s="25"/>
+      <c r="Q118" s="25"/>
+      <c r="R118" s="25"/>
+      <c r="S118" s="25"/>
+      <c r="T118" s="25"/>
+      <c r="U118" s="25"/>
+      <c r="V118" s="25"/>
+      <c r="W118" s="25"/>
+      <c r="X118" s="25"/>
+      <c r="Y118" s="25"/>
+      <c r="Z118" s="25"/>
+      <c r="AA118" s="25"/>
+      <c r="AB118" s="25"/>
+      <c r="AC118" s="25"/>
+      <c r="AD118" s="25"/>
+      <c r="AE118" s="25"/>
+      <c r="AF118" s="25"/>
+      <c r="AG118" s="25"/>
+      <c r="AH118" s="25"/>
+      <c r="AI118" s="25"/>
+    </row>
+    <row r="119" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A119" s="25"/>
+      <c r="B119" s="66"/>
+      <c r="C119" s="66"/>
+      <c r="D119" s="25"/>
+      <c r="E119" s="25"/>
+      <c r="F119" s="25"/>
+      <c r="G119" s="25"/>
+      <c r="H119" s="25"/>
+      <c r="I119" s="25"/>
+      <c r="J119" s="25"/>
+      <c r="K119" s="25"/>
+      <c r="L119" s="25"/>
+      <c r="M119" s="25"/>
+      <c r="N119" s="25"/>
+      <c r="O119" s="25"/>
+      <c r="P119" s="25"/>
+      <c r="Q119" s="25"/>
+      <c r="R119" s="25"/>
+      <c r="S119" s="25"/>
+      <c r="T119" s="25"/>
+      <c r="U119" s="25"/>
+      <c r="V119" s="25"/>
+      <c r="W119" s="25"/>
+      <c r="X119" s="25"/>
+      <c r="Y119" s="25"/>
+      <c r="Z119" s="25"/>
+      <c r="AA119" s="25"/>
+      <c r="AB119" s="25"/>
+      <c r="AC119" s="25"/>
+      <c r="AD119" s="25"/>
+      <c r="AE119" s="25"/>
+      <c r="AF119" s="25"/>
+      <c r="AG119" s="25"/>
+      <c r="AH119" s="25"/>
+      <c r="AI119" s="25"/>
+      <c r="AJ119" s="66"/>
+    </row>
+    <row r="120" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A120" s="25"/>
+      <c r="B120" s="66"/>
+      <c r="C120" s="66"/>
+      <c r="D120" s="25"/>
+      <c r="E120" s="25"/>
+      <c r="F120" s="25"/>
+      <c r="G120" s="25"/>
+      <c r="H120" s="25"/>
+      <c r="I120" s="25"/>
+      <c r="J120" s="25"/>
+      <c r="K120" s="25"/>
+      <c r="L120" s="25"/>
+      <c r="M120" s="25"/>
+      <c r="N120" s="25"/>
+      <c r="O120" s="25"/>
+      <c r="P120" s="25"/>
+      <c r="Q120" s="25"/>
+      <c r="R120" s="25"/>
+      <c r="S120" s="25"/>
+      <c r="T120" s="25"/>
+      <c r="U120" s="25"/>
+      <c r="V120" s="25"/>
+      <c r="W120" s="25"/>
+      <c r="X120" s="25"/>
+      <c r="Y120" s="25"/>
+      <c r="Z120" s="25"/>
+      <c r="AA120" s="25"/>
+      <c r="AB120" s="25"/>
+      <c r="AC120" s="25"/>
+      <c r="AD120" s="25"/>
+      <c r="AE120" s="25"/>
+      <c r="AF120" s="25"/>
+      <c r="AG120" s="25"/>
+      <c r="AH120" s="25"/>
+      <c r="AI120" s="25"/>
+    </row>
+    <row r="121" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A121" s="25"/>
+      <c r="B121" s="66"/>
+      <c r="C121" s="66"/>
+      <c r="D121" s="25"/>
+      <c r="E121" s="25"/>
+      <c r="F121" s="25"/>
+      <c r="G121" s="25"/>
+      <c r="H121" s="25"/>
+      <c r="I121" s="25"/>
+      <c r="J121" s="25"/>
+      <c r="K121" s="25"/>
+      <c r="L121" s="25"/>
+      <c r="M121" s="25"/>
+      <c r="N121" s="25"/>
+      <c r="O121" s="25"/>
+      <c r="P121" s="25"/>
+      <c r="Q121" s="25"/>
+      <c r="R121" s="25"/>
+      <c r="S121" s="25"/>
+      <c r="T121" s="25"/>
+      <c r="U121" s="25"/>
+      <c r="V121" s="25"/>
+      <c r="W121" s="25"/>
+      <c r="X121" s="25"/>
+      <c r="Y121" s="25"/>
+      <c r="Z121" s="25"/>
+      <c r="AA121" s="25"/>
+      <c r="AB121" s="25"/>
+      <c r="AC121" s="25"/>
+      <c r="AD121" s="25"/>
+      <c r="AE121" s="25"/>
+      <c r="AF121" s="25"/>
+      <c r="AG121" s="25"/>
+      <c r="AH121" s="25"/>
+      <c r="AI121" s="25"/>
+    </row>
+    <row r="122" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A122" s="25"/>
+      <c r="B122" s="66"/>
+      <c r="C122" s="66"/>
+      <c r="D122" s="25"/>
+      <c r="E122" s="25"/>
+      <c r="F122" s="25"/>
+      <c r="G122" s="25"/>
+      <c r="H122" s="25"/>
+      <c r="I122" s="25"/>
+      <c r="J122" s="25"/>
+      <c r="K122" s="25"/>
+      <c r="L122" s="25"/>
+      <c r="M122" s="25"/>
+      <c r="N122" s="25"/>
+      <c r="O122" s="25"/>
+      <c r="P122" s="25"/>
+      <c r="Q122" s="25"/>
+      <c r="R122" s="25"/>
+      <c r="S122" s="25"/>
+      <c r="T122" s="25"/>
+      <c r="U122" s="25"/>
+      <c r="V122" s="25"/>
+      <c r="W122" s="25"/>
+      <c r="X122" s="25"/>
+      <c r="Y122" s="25"/>
+      <c r="Z122" s="25"/>
+      <c r="AA122" s="25"/>
+      <c r="AB122" s="25"/>
+      <c r="AC122" s="25"/>
+      <c r="AD122" s="25"/>
+      <c r="AE122" s="25"/>
+      <c r="AF122" s="25"/>
+      <c r="AG122" s="25"/>
+      <c r="AH122" s="25"/>
+      <c r="AI122" s="25"/>
+    </row>
+    <row r="123" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A123" s="25"/>
+      <c r="B123" s="66"/>
+      <c r="C123" s="66"/>
+      <c r="D123" s="25"/>
+      <c r="E123" s="25"/>
+      <c r="F123" s="25"/>
+      <c r="G123" s="25"/>
+      <c r="H123" s="25"/>
+      <c r="I123" s="25"/>
+      <c r="J123" s="25"/>
+      <c r="K123" s="25"/>
+      <c r="L123" s="25"/>
+      <c r="M123" s="25"/>
+      <c r="N123" s="25"/>
+      <c r="O123" s="25"/>
+      <c r="P123" s="25"/>
+      <c r="Q123" s="25"/>
+      <c r="R123" s="25"/>
+      <c r="S123" s="25"/>
+      <c r="T123" s="25"/>
+      <c r="U123" s="25"/>
+      <c r="V123" s="25"/>
+      <c r="W123" s="25"/>
+      <c r="X123" s="25"/>
+      <c r="Y123" s="25"/>
+      <c r="Z123" s="25"/>
+      <c r="AA123" s="25"/>
+      <c r="AB123" s="25"/>
+      <c r="AC123" s="25"/>
+      <c r="AD123" s="25"/>
+      <c r="AE123" s="25"/>
+      <c r="AF123" s="25"/>
+      <c r="AG123" s="25"/>
+      <c r="AH123" s="25"/>
+      <c r="AI123" s="25"/>
+    </row>
+    <row r="124" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A124" s="25"/>
+      <c r="B124" s="66"/>
+      <c r="C124" s="66"/>
+      <c r="D124" s="25"/>
+      <c r="E124" s="25"/>
+      <c r="F124" s="25"/>
+      <c r="G124" s="25"/>
+      <c r="H124" s="25"/>
+      <c r="I124" s="25"/>
+      <c r="J124" s="25"/>
+      <c r="K124" s="25"/>
+      <c r="L124" s="25"/>
+      <c r="M124" s="25"/>
+      <c r="N124" s="25"/>
+      <c r="O124" s="25"/>
+      <c r="P124" s="25"/>
+      <c r="Q124" s="25"/>
+      <c r="R124" s="25"/>
+      <c r="S124" s="25"/>
+      <c r="T124" s="25"/>
+      <c r="U124" s="25"/>
+      <c r="V124" s="25"/>
+      <c r="W124" s="25"/>
+      <c r="X124" s="25"/>
+      <c r="Y124" s="25"/>
+      <c r="Z124" s="25"/>
+      <c r="AA124" s="25"/>
+      <c r="AB124" s="25"/>
+      <c r="AC124" s="25"/>
+      <c r="AD124" s="25"/>
+      <c r="AE124" s="25"/>
+      <c r="AF124" s="25"/>
+      <c r="AG124" s="25"/>
+      <c r="AH124" s="25"/>
+      <c r="AI124" s="25"/>
+    </row>
+    <row r="125" spans="1:36" ht="18" x14ac:dyDescent="0.3">
+      <c r="A125" s="60" t="s">
+        <v>110</v>
+      </c>
+      <c r="B125" s="61"/>
+      <c r="C125" s="61"/>
+      <c r="D125" s="61"/>
+      <c r="E125" s="61"/>
+      <c r="F125" s="61"/>
+      <c r="G125" s="61"/>
+      <c r="H125" s="61"/>
+      <c r="I125" s="61"/>
+      <c r="J125" s="61"/>
+      <c r="K125" s="61"/>
+      <c r="L125" s="61"/>
+      <c r="M125" s="61"/>
+      <c r="N125" s="61"/>
+      <c r="O125" s="61"/>
+      <c r="P125" s="61"/>
+      <c r="Q125" s="61"/>
+      <c r="R125" s="61"/>
+      <c r="S125" s="61"/>
+      <c r="T125" s="61"/>
+      <c r="U125" s="61"/>
+      <c r="V125" s="61"/>
+      <c r="W125" s="61"/>
+      <c r="X125" s="61"/>
+      <c r="Y125" s="61"/>
+      <c r="Z125" s="61"/>
+      <c r="AA125" s="61"/>
+      <c r="AB125" s="61"/>
+      <c r="AC125" s="61"/>
+      <c r="AD125" s="61"/>
+      <c r="AE125" s="61"/>
+      <c r="AF125" s="61"/>
+      <c r="AG125" s="61"/>
+      <c r="AH125" s="61"/>
+      <c r="AI125" s="61"/>
+      <c r="AJ125" s="61"/>
+    </row>
+    <row r="126" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A126" s="72"/>
+      <c r="B126" s="62" t="s">
+        <v>109</v>
+      </c>
+      <c r="C126" s="63" t="s">
+        <v>4</v>
+      </c>
+      <c r="D126" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="E126" s="64">
+        <v>1</v>
+      </c>
+      <c r="F126" s="64">
+        <v>2</v>
+      </c>
+      <c r="G126" s="64">
+        <v>3</v>
+      </c>
+      <c r="H126" s="64">
+        <v>4</v>
+      </c>
+      <c r="I126" s="64">
+        <v>5</v>
+      </c>
+      <c r="J126" s="64">
+        <v>6</v>
+      </c>
+      <c r="K126" s="64">
+        <v>7</v>
+      </c>
+      <c r="L126" s="64">
+        <v>8</v>
+      </c>
+      <c r="M126" s="64">
+        <v>9</v>
+      </c>
+      <c r="N126" s="64">
+        <v>10</v>
+      </c>
+      <c r="O126" s="64">
+        <v>11</v>
+      </c>
+      <c r="P126" s="64">
+        <v>12</v>
+      </c>
+      <c r="Q126" s="64">
+        <v>13</v>
+      </c>
+      <c r="R126" s="64">
+        <v>14</v>
+      </c>
+      <c r="S126" s="64">
+        <v>15</v>
+      </c>
+      <c r="T126" s="64">
+        <v>16</v>
+      </c>
+      <c r="U126" s="64">
+        <v>17</v>
+      </c>
+      <c r="V126" s="64">
+        <v>18</v>
+      </c>
+      <c r="W126" s="64">
+        <v>19</v>
+      </c>
+      <c r="X126" s="64">
+        <v>20</v>
+      </c>
+      <c r="Y126" s="64">
+        <v>21</v>
+      </c>
+      <c r="Z126" s="64">
+        <v>22</v>
+      </c>
+      <c r="AA126" s="64">
+        <v>23</v>
+      </c>
+      <c r="AB126" s="64">
+        <v>24</v>
+      </c>
+      <c r="AC126" s="64">
+        <v>25</v>
+      </c>
+      <c r="AD126" s="64">
+        <v>26</v>
+      </c>
+      <c r="AE126" s="64">
+        <v>27</v>
+      </c>
+      <c r="AF126" s="64">
+        <v>28</v>
+      </c>
+      <c r="AG126" s="64">
+        <v>29</v>
+      </c>
+      <c r="AH126" s="64">
+        <v>30</v>
+      </c>
+      <c r="AI126" s="64">
+        <v>31</v>
+      </c>
+      <c r="AJ126" s="65" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A127" s="25"/>
+      <c r="B127" s="66"/>
+      <c r="C127" s="66"/>
+      <c r="D127" s="25"/>
+      <c r="E127" s="25"/>
+      <c r="F127" s="25"/>
+      <c r="G127" s="25"/>
+      <c r="H127" s="25"/>
+      <c r="I127" s="25"/>
+      <c r="J127" s="25"/>
+      <c r="K127" s="25"/>
+      <c r="L127" s="25"/>
+      <c r="M127" s="25"/>
+      <c r="N127" s="25"/>
+      <c r="O127" s="25"/>
+      <c r="P127" s="25"/>
+      <c r="Q127" s="25"/>
+      <c r="R127" s="25"/>
+      <c r="S127" s="25"/>
+      <c r="T127" s="25"/>
+      <c r="U127" s="25"/>
+      <c r="V127" s="25"/>
+      <c r="W127" s="25"/>
+      <c r="X127" s="25"/>
+      <c r="Y127" s="25"/>
+      <c r="Z127" s="25"/>
+      <c r="AA127" s="25"/>
+      <c r="AB127" s="25"/>
+      <c r="AC127" s="25"/>
+      <c r="AD127" s="25"/>
+      <c r="AE127" s="25"/>
+      <c r="AF127" s="25"/>
+      <c r="AG127" s="25"/>
+      <c r="AH127" s="25"/>
+      <c r="AI127" s="25"/>
+    </row>
+    <row r="128" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A128" s="25"/>
+      <c r="B128" s="66"/>
+      <c r="C128" s="66"/>
+      <c r="D128" s="25"/>
+      <c r="E128" s="25"/>
+      <c r="F128" s="25"/>
+      <c r="G128" s="25"/>
+      <c r="H128" s="25"/>
+      <c r="I128" s="25"/>
+      <c r="J128" s="25"/>
+      <c r="K128" s="25"/>
+      <c r="L128" s="25"/>
+      <c r="M128" s="25"/>
+      <c r="N128" s="25"/>
+      <c r="O128" s="25"/>
+      <c r="P128" s="25"/>
+      <c r="Q128" s="25"/>
+      <c r="R128" s="25"/>
+      <c r="S128" s="25"/>
+      <c r="T128" s="25"/>
+      <c r="U128" s="25"/>
+      <c r="V128" s="25"/>
+      <c r="W128" s="25"/>
+      <c r="X128" s="25"/>
+      <c r="Y128" s="25"/>
+      <c r="Z128" s="25"/>
+      <c r="AA128" s="25"/>
+      <c r="AB128" s="25"/>
+      <c r="AC128" s="25"/>
+      <c r="AD128" s="25"/>
+      <c r="AE128" s="25"/>
+      <c r="AF128" s="25"/>
+      <c r="AG128" s="25"/>
+      <c r="AH128" s="25"/>
+      <c r="AI128" s="25"/>
+    </row>
+    <row r="129" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A129" s="25"/>
+      <c r="B129" s="66"/>
+      <c r="C129" s="66"/>
+      <c r="D129" s="25"/>
+      <c r="E129" s="25"/>
+      <c r="F129" s="25"/>
+      <c r="G129" s="25"/>
+      <c r="H129" s="25"/>
+      <c r="I129" s="25"/>
+      <c r="J129" s="25"/>
+      <c r="K129" s="25"/>
+      <c r="L129" s="25"/>
+      <c r="M129" s="25"/>
+      <c r="N129" s="25"/>
+      <c r="O129" s="25"/>
+      <c r="P129" s="25"/>
+      <c r="Q129" s="25"/>
+      <c r="R129" s="25"/>
+      <c r="S129" s="25"/>
+      <c r="T129" s="25"/>
+      <c r="U129" s="25"/>
+      <c r="V129" s="25"/>
+      <c r="W129" s="25"/>
+      <c r="X129" s="25"/>
+      <c r="Y129" s="25"/>
+      <c r="Z129" s="25"/>
+      <c r="AA129" s="25"/>
+      <c r="AB129" s="25"/>
+      <c r="AC129" s="25"/>
+      <c r="AD129" s="25"/>
+      <c r="AE129" s="25"/>
+      <c r="AF129" s="25"/>
+      <c r="AG129" s="25"/>
+      <c r="AH129" s="25"/>
+      <c r="AI129" s="25"/>
+    </row>
+    <row r="130" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A130" s="25"/>
+      <c r="B130" s="66"/>
+      <c r="C130" s="66"/>
+      <c r="D130" s="25"/>
+      <c r="E130" s="25"/>
+      <c r="F130" s="25"/>
+      <c r="G130" s="25"/>
+      <c r="H130" s="25"/>
+      <c r="I130" s="25"/>
+      <c r="J130" s="25"/>
+      <c r="K130" s="25"/>
+      <c r="L130" s="25"/>
+      <c r="M130" s="25"/>
+      <c r="N130" s="25"/>
+      <c r="O130" s="25"/>
+      <c r="P130" s="25"/>
+      <c r="Q130" s="25"/>
+      <c r="R130" s="25"/>
+      <c r="S130" s="25"/>
+      <c r="T130" s="25"/>
+      <c r="U130" s="25"/>
+      <c r="V130" s="25"/>
+      <c r="W130" s="25"/>
+      <c r="X130" s="25"/>
+      <c r="Y130" s="25"/>
+      <c r="Z130" s="25"/>
+      <c r="AA130" s="25"/>
+      <c r="AB130" s="25"/>
+      <c r="AC130" s="25"/>
+      <c r="AD130" s="25"/>
+      <c r="AE130" s="25"/>
+      <c r="AF130" s="25"/>
+      <c r="AG130" s="25"/>
+      <c r="AH130" s="25"/>
+      <c r="AI130" s="25"/>
+    </row>
+    <row r="131" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A131" s="25"/>
+      <c r="B131" s="66"/>
+      <c r="C131" s="66"/>
+      <c r="D131" s="25"/>
+      <c r="E131" s="25"/>
+      <c r="F131" s="25"/>
+      <c r="G131" s="25"/>
+      <c r="H131" s="25"/>
+      <c r="I131" s="25"/>
+      <c r="J131" s="25"/>
+      <c r="K131" s="25"/>
+      <c r="L131" s="25"/>
+      <c r="M131" s="25"/>
+      <c r="N131" s="25"/>
+      <c r="O131" s="25"/>
+      <c r="P131" s="25"/>
+      <c r="Q131" s="25"/>
+      <c r="R131" s="25"/>
+      <c r="S131" s="25"/>
+      <c r="T131" s="25"/>
+      <c r="U131" s="25"/>
+      <c r="V131" s="25"/>
+      <c r="W131" s="25"/>
+      <c r="X131" s="25"/>
+      <c r="Y131" s="25"/>
+      <c r="Z131" s="25"/>
+      <c r="AA131" s="25"/>
+      <c r="AB131" s="25"/>
+      <c r="AC131" s="25"/>
+      <c r="AD131" s="25"/>
+      <c r="AE131" s="25"/>
+      <c r="AF131" s="25"/>
+      <c r="AG131" s="25"/>
+      <c r="AH131" s="25"/>
+      <c r="AI131" s="25"/>
+    </row>
+    <row r="132" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A132" s="25"/>
+      <c r="B132" s="66"/>
+      <c r="C132" s="66"/>
+      <c r="D132" s="25"/>
+      <c r="E132" s="25"/>
+      <c r="F132" s="25"/>
+      <c r="G132" s="25"/>
+      <c r="H132" s="25"/>
+      <c r="I132" s="25"/>
+      <c r="J132" s="25"/>
+      <c r="K132" s="25"/>
+      <c r="L132" s="25"/>
+      <c r="M132" s="25"/>
+      <c r="N132" s="25"/>
+      <c r="O132" s="25"/>
+      <c r="P132" s="25"/>
+      <c r="Q132" s="25"/>
+      <c r="R132" s="25"/>
+      <c r="S132" s="25"/>
+      <c r="T132" s="25"/>
+      <c r="U132" s="25"/>
+      <c r="V132" s="25"/>
+      <c r="W132" s="25"/>
+      <c r="X132" s="25"/>
+      <c r="Y132" s="25"/>
+      <c r="Z132" s="25"/>
+      <c r="AA132" s="25"/>
+      <c r="AB132" s="25"/>
+      <c r="AC132" s="25"/>
+      <c r="AD132" s="25"/>
+      <c r="AE132" s="25"/>
+      <c r="AF132" s="25"/>
+      <c r="AG132" s="25"/>
+      <c r="AH132" s="25"/>
+      <c r="AI132" s="25"/>
+    </row>
+    <row r="133" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A133" s="25"/>
+      <c r="B133" s="66"/>
+      <c r="C133" s="66"/>
+      <c r="D133" s="25"/>
+      <c r="E133" s="25"/>
+      <c r="F133" s="25"/>
+      <c r="G133" s="25"/>
+      <c r="H133" s="25"/>
+      <c r="I133" s="25"/>
+      <c r="J133" s="25"/>
+      <c r="K133" s="25"/>
+      <c r="L133" s="25"/>
+      <c r="M133" s="25"/>
+      <c r="N133" s="25"/>
+      <c r="O133" s="25"/>
+      <c r="P133" s="25"/>
+      <c r="Q133" s="25"/>
+      <c r="R133" s="25"/>
+      <c r="S133" s="25"/>
+      <c r="T133" s="25"/>
+      <c r="U133" s="25"/>
+      <c r="V133" s="25"/>
+      <c r="W133" s="25"/>
+      <c r="X133" s="25"/>
+      <c r="Y133" s="25"/>
+      <c r="Z133" s="25"/>
+      <c r="AA133" s="25"/>
+      <c r="AB133" s="25"/>
+      <c r="AC133" s="25"/>
+      <c r="AD133" s="25"/>
+      <c r="AE133" s="25"/>
+      <c r="AF133" s="25"/>
+      <c r="AG133" s="25"/>
+      <c r="AH133" s="25"/>
+      <c r="AI133" s="25"/>
+    </row>
+    <row r="134" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A134" s="25"/>
+      <c r="B134" s="66"/>
+      <c r="C134" s="66"/>
+      <c r="D134" s="25"/>
+      <c r="E134" s="25"/>
+      <c r="F134" s="25"/>
+      <c r="G134" s="25"/>
+      <c r="H134" s="25"/>
+      <c r="I134" s="25"/>
+      <c r="J134" s="25"/>
+      <c r="K134" s="25"/>
+      <c r="L134" s="25"/>
+      <c r="M134" s="25"/>
+      <c r="N134" s="25"/>
+      <c r="O134" s="25"/>
+      <c r="P134" s="25"/>
+      <c r="Q134" s="25"/>
+      <c r="R134" s="25"/>
+      <c r="S134" s="25"/>
+      <c r="T134" s="25"/>
+      <c r="U134" s="25"/>
+      <c r="V134" s="25"/>
+      <c r="W134" s="25"/>
+      <c r="X134" s="25"/>
+      <c r="Y134" s="25"/>
+      <c r="Z134" s="25"/>
+      <c r="AA134" s="25"/>
+      <c r="AB134" s="25"/>
+      <c r="AC134" s="25"/>
+      <c r="AD134" s="25"/>
+      <c r="AE134" s="25"/>
+      <c r="AF134" s="25"/>
+      <c r="AG134" s="25"/>
+      <c r="AH134" s="25"/>
+      <c r="AI134" s="25"/>
+    </row>
+    <row r="135" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A135" s="25"/>
+      <c r="B135" s="66"/>
+      <c r="C135" s="66"/>
+      <c r="D135" s="25"/>
+      <c r="E135" s="25"/>
+      <c r="F135" s="25"/>
+      <c r="G135" s="25"/>
+      <c r="H135" s="25"/>
+      <c r="I135" s="25"/>
+      <c r="J135" s="25"/>
+      <c r="K135" s="25"/>
+      <c r="L135" s="25"/>
+      <c r="M135" s="25"/>
+      <c r="N135" s="25"/>
+      <c r="O135" s="25"/>
+      <c r="P135" s="25"/>
+      <c r="Q135" s="25"/>
+      <c r="R135" s="25"/>
+      <c r="S135" s="25"/>
+      <c r="T135" s="25"/>
+      <c r="U135" s="25"/>
+      <c r="V135" s="25"/>
+      <c r="W135" s="25"/>
+      <c r="X135" s="25"/>
+      <c r="Y135" s="25"/>
+      <c r="Z135" s="25"/>
+      <c r="AA135" s="25"/>
+      <c r="AB135" s="25"/>
+      <c r="AC135" s="25"/>
+      <c r="AD135" s="25"/>
+      <c r="AE135" s="25"/>
+      <c r="AF135" s="25"/>
+      <c r="AG135" s="25"/>
+      <c r="AH135" s="25"/>
+      <c r="AI135" s="25"/>
+    </row>
+    <row r="136" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A136" s="25"/>
+      <c r="B136" s="66"/>
+      <c r="C136" s="66"/>
+      <c r="D136" s="25"/>
+      <c r="E136" s="25"/>
+      <c r="F136" s="25"/>
+      <c r="G136" s="25"/>
+      <c r="H136" s="25"/>
+      <c r="I136" s="25"/>
+      <c r="J136" s="25"/>
+      <c r="K136" s="25"/>
+      <c r="L136" s="25"/>
+      <c r="M136" s="25"/>
+      <c r="N136" s="25"/>
+      <c r="O136" s="25"/>
+      <c r="P136" s="25"/>
+      <c r="Q136" s="25"/>
+      <c r="R136" s="25"/>
+      <c r="S136" s="25"/>
+      <c r="T136" s="25"/>
+      <c r="U136" s="25"/>
+      <c r="V136" s="25"/>
+      <c r="W136" s="25"/>
+      <c r="X136" s="25"/>
+      <c r="Y136" s="25"/>
+      <c r="Z136" s="25"/>
+      <c r="AA136" s="25"/>
+      <c r="AB136" s="25"/>
+      <c r="AC136" s="25"/>
+      <c r="AD136" s="25"/>
+      <c r="AE136" s="25"/>
+      <c r="AF136" s="25"/>
+      <c r="AG136" s="25"/>
+      <c r="AH136" s="25"/>
+      <c r="AI136" s="25"/>
+    </row>
+    <row r="137" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A137" s="25"/>
+      <c r="B137" s="66"/>
+      <c r="C137" s="66"/>
+      <c r="D137" s="25"/>
+      <c r="E137" s="25"/>
+      <c r="F137" s="25"/>
+      <c r="G137" s="25"/>
+      <c r="H137" s="25"/>
+      <c r="I137" s="25"/>
+      <c r="J137" s="25"/>
+      <c r="K137" s="25"/>
+      <c r="L137" s="25"/>
+      <c r="M137" s="25"/>
+      <c r="N137" s="25"/>
+      <c r="O137" s="25"/>
+      <c r="P137" s="25"/>
+      <c r="Q137" s="25"/>
+      <c r="R137" s="25"/>
+      <c r="S137" s="25"/>
+      <c r="T137" s="25"/>
+      <c r="U137" s="25"/>
+      <c r="V137" s="25"/>
+      <c r="W137" s="25"/>
+      <c r="X137" s="25"/>
+      <c r="Y137" s="25"/>
+      <c r="Z137" s="25"/>
+      <c r="AA137" s="25"/>
+      <c r="AB137" s="25"/>
+      <c r="AC137" s="25"/>
+      <c r="AD137" s="25"/>
+      <c r="AE137" s="25"/>
+      <c r="AF137" s="25"/>
+      <c r="AG137" s="25"/>
+      <c r="AH137" s="25"/>
+      <c r="AI137" s="25"/>
+    </row>
+    <row r="138" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A138" s="25"/>
+      <c r="B138" s="66"/>
+      <c r="C138" s="66"/>
+      <c r="D138" s="25"/>
+      <c r="E138" s="25"/>
+      <c r="F138" s="25"/>
+      <c r="G138" s="25"/>
+      <c r="H138" s="25"/>
+      <c r="I138" s="25"/>
+      <c r="J138" s="25"/>
+      <c r="K138" s="25"/>
+      <c r="L138" s="25"/>
+      <c r="M138" s="25"/>
+      <c r="N138" s="25"/>
+      <c r="O138" s="25"/>
+      <c r="P138" s="25"/>
+      <c r="Q138" s="25"/>
+      <c r="R138" s="25"/>
+      <c r="S138" s="25"/>
+      <c r="T138" s="25"/>
+      <c r="U138" s="25"/>
+      <c r="V138" s="25"/>
+      <c r="W138" s="25"/>
+      <c r="X138" s="25"/>
+      <c r="Y138" s="25"/>
+      <c r="Z138" s="25"/>
+      <c r="AA138" s="25"/>
+      <c r="AB138" s="25"/>
+      <c r="AC138" s="25"/>
+      <c r="AD138" s="25"/>
+      <c r="AE138" s="25"/>
+      <c r="AF138" s="25"/>
+      <c r="AG138" s="25"/>
+      <c r="AH138" s="25"/>
+      <c r="AI138" s="25"/>
+    </row>
+    <row r="139" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A139" s="25"/>
+      <c r="B139" s="66"/>
+      <c r="C139" s="66"/>
+      <c r="D139" s="25"/>
+      <c r="E139" s="25"/>
+      <c r="F139" s="25"/>
+      <c r="G139" s="25"/>
+      <c r="H139" s="25"/>
+      <c r="I139" s="25"/>
+      <c r="J139" s="25"/>
+      <c r="K139" s="25"/>
+      <c r="L139" s="25"/>
+      <c r="M139" s="25"/>
+      <c r="N139" s="25"/>
+      <c r="O139" s="25"/>
+      <c r="P139" s="25"/>
+      <c r="Q139" s="25"/>
+      <c r="R139" s="25"/>
+      <c r="S139" s="25"/>
+      <c r="T139" s="25"/>
+      <c r="U139" s="25"/>
+      <c r="V139" s="25"/>
+      <c r="W139" s="25"/>
+      <c r="X139" s="25"/>
+      <c r="Y139" s="25"/>
+      <c r="Z139" s="25"/>
+      <c r="AA139" s="25"/>
+      <c r="AB139" s="25"/>
+      <c r="AC139" s="25"/>
+      <c r="AD139" s="25"/>
+      <c r="AE139" s="25"/>
+      <c r="AF139" s="25"/>
+      <c r="AG139" s="25"/>
+      <c r="AH139" s="25"/>
+      <c r="AI139" s="25"/>
+    </row>
+    <row r="140" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A140" s="25"/>
+      <c r="B140" s="66"/>
+      <c r="C140" s="66"/>
+      <c r="D140" s="25"/>
+      <c r="E140" s="25"/>
+      <c r="F140" s="25"/>
+      <c r="G140" s="25"/>
+      <c r="H140" s="25"/>
+      <c r="I140" s="25"/>
+      <c r="J140" s="25"/>
+      <c r="K140" s="25"/>
+      <c r="L140" s="25"/>
+      <c r="M140" s="25"/>
+      <c r="N140" s="25"/>
+      <c r="O140" s="25"/>
+      <c r="P140" s="25"/>
+      <c r="Q140" s="25"/>
+      <c r="R140" s="25"/>
+      <c r="S140" s="25"/>
+      <c r="T140" s="25"/>
+      <c r="U140" s="25"/>
+      <c r="V140" s="25"/>
+      <c r="W140" s="25"/>
+      <c r="X140" s="25"/>
+      <c r="Y140" s="25"/>
+      <c r="Z140" s="25"/>
+      <c r="AA140" s="25"/>
+      <c r="AB140" s="25"/>
+      <c r="AC140" s="25"/>
+      <c r="AD140" s="25"/>
+      <c r="AE140" s="25"/>
+      <c r="AF140" s="25"/>
+      <c r="AG140" s="25"/>
+      <c r="AH140" s="25"/>
+      <c r="AI140" s="25"/>
+    </row>
+    <row r="141" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A141" s="25"/>
+      <c r="B141" s="66"/>
+      <c r="C141" s="66"/>
+      <c r="D141" s="25"/>
+      <c r="E141" s="25"/>
+      <c r="F141" s="25"/>
+      <c r="G141" s="25"/>
+      <c r="H141" s="25"/>
+      <c r="I141" s="25"/>
+      <c r="J141" s="25"/>
+      <c r="K141" s="25"/>
+      <c r="L141" s="25"/>
+      <c r="M141" s="25"/>
+      <c r="N141" s="25"/>
+      <c r="O141" s="25"/>
+      <c r="P141" s="25"/>
+      <c r="Q141" s="25"/>
+      <c r="R141" s="25"/>
+      <c r="S141" s="25"/>
+      <c r="T141" s="25"/>
+      <c r="U141" s="25"/>
+      <c r="V141" s="25"/>
+      <c r="W141" s="25"/>
+      <c r="X141" s="25"/>
+      <c r="Y141" s="25"/>
+      <c r="Z141" s="25"/>
+      <c r="AA141" s="25"/>
+      <c r="AB141" s="25"/>
+      <c r="AC141" s="25"/>
+      <c r="AD141" s="25"/>
+      <c r="AE141" s="25"/>
+      <c r="AF141" s="25"/>
+      <c r="AG141" s="25"/>
+      <c r="AH141" s="25"/>
+      <c r="AI141" s="25"/>
+    </row>
+    <row r="142" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A142" s="25"/>
+      <c r="B142" s="66"/>
+      <c r="C142" s="66"/>
+      <c r="D142" s="25"/>
+      <c r="E142" s="25"/>
+      <c r="F142" s="25"/>
+      <c r="G142" s="25"/>
+      <c r="H142" s="25"/>
+      <c r="I142" s="25"/>
+      <c r="J142" s="25"/>
+      <c r="K142" s="25"/>
+      <c r="L142" s="25"/>
+      <c r="M142" s="25"/>
+      <c r="N142" s="25"/>
+      <c r="O142" s="25"/>
+      <c r="P142" s="25"/>
+      <c r="Q142" s="25"/>
+      <c r="R142" s="25"/>
+      <c r="S142" s="25"/>
+      <c r="T142" s="25"/>
+      <c r="U142" s="25"/>
+      <c r="V142" s="25"/>
+      <c r="W142" s="25"/>
+      <c r="X142" s="25"/>
+      <c r="Y142" s="25"/>
+      <c r="Z142" s="25"/>
+      <c r="AA142" s="25"/>
+      <c r="AB142" s="25"/>
+      <c r="AC142" s="25"/>
+      <c r="AD142" s="25"/>
+      <c r="AE142" s="25"/>
+      <c r="AF142" s="25"/>
+      <c r="AG142" s="25"/>
+      <c r="AH142" s="25"/>
+      <c r="AI142" s="25"/>
+    </row>
+    <row r="143" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A143" s="25"/>
+      <c r="B143" s="66"/>
+      <c r="C143" s="66"/>
+      <c r="D143" s="25"/>
+      <c r="E143" s="25"/>
+      <c r="F143" s="25"/>
+      <c r="G143" s="25"/>
+      <c r="H143" s="25"/>
+      <c r="I143" s="25"/>
+      <c r="J143" s="25"/>
+      <c r="K143" s="25"/>
+      <c r="L143" s="25"/>
+      <c r="M143" s="25"/>
+      <c r="N143" s="25"/>
+      <c r="O143" s="25"/>
+      <c r="P143" s="25"/>
+      <c r="Q143" s="25"/>
+      <c r="R143" s="25"/>
+      <c r="S143" s="25"/>
+      <c r="T143" s="25"/>
+      <c r="U143" s="25"/>
+      <c r="V143" s="25"/>
+      <c r="W143" s="25"/>
+      <c r="X143" s="25"/>
+      <c r="Y143" s="25"/>
+      <c r="Z143" s="25"/>
+      <c r="AA143" s="25"/>
+      <c r="AB143" s="25"/>
+      <c r="AC143" s="25"/>
+      <c r="AD143" s="25"/>
+      <c r="AE143" s="25"/>
+      <c r="AF143" s="25"/>
+      <c r="AG143" s="25"/>
+      <c r="AH143" s="25"/>
+      <c r="AI143" s="25"/>
+    </row>
+    <row r="144" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A144" s="25"/>
+      <c r="B144" s="66"/>
+      <c r="C144" s="66"/>
+      <c r="D144" s="25"/>
+      <c r="E144" s="25"/>
+      <c r="F144" s="25"/>
+      <c r="G144" s="25"/>
+      <c r="H144" s="25"/>
+      <c r="I144" s="25"/>
+      <c r="J144" s="25"/>
+      <c r="K144" s="25"/>
+      <c r="L144" s="25"/>
+      <c r="M144" s="25"/>
+      <c r="N144" s="25"/>
+      <c r="O144" s="25"/>
+      <c r="P144" s="25"/>
+      <c r="Q144" s="25"/>
+      <c r="R144" s="25"/>
+      <c r="S144" s="25"/>
+      <c r="T144" s="25"/>
+      <c r="U144" s="25"/>
+      <c r="V144" s="25"/>
+      <c r="W144" s="25"/>
+      <c r="X144" s="25"/>
+      <c r="Y144" s="25"/>
+      <c r="Z144" s="25"/>
+      <c r="AA144" s="25"/>
+      <c r="AB144" s="25"/>
+      <c r="AC144" s="25"/>
+      <c r="AD144" s="25"/>
+      <c r="AE144" s="25"/>
+      <c r="AF144" s="25"/>
+      <c r="AG144" s="25"/>
+      <c r="AH144" s="25"/>
+      <c r="AI144" s="25"/>
+    </row>
+    <row r="145" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A145" s="25"/>
+      <c r="B145" s="66"/>
+      <c r="C145" s="66"/>
+      <c r="D145" s="25"/>
+      <c r="E145" s="25"/>
+      <c r="F145" s="25"/>
+      <c r="G145" s="25"/>
+      <c r="H145" s="25"/>
+      <c r="I145" s="25"/>
+      <c r="J145" s="25"/>
+      <c r="K145" s="25"/>
+      <c r="L145" s="25"/>
+      <c r="M145" s="25"/>
+      <c r="N145" s="25"/>
+      <c r="O145" s="25"/>
+      <c r="P145" s="25"/>
+      <c r="Q145" s="25"/>
+      <c r="R145" s="25"/>
+      <c r="S145" s="25"/>
+      <c r="T145" s="25"/>
+      <c r="U145" s="25"/>
+      <c r="V145" s="25"/>
+      <c r="W145" s="25"/>
+      <c r="X145" s="25"/>
+      <c r="Y145" s="25"/>
+      <c r="Z145" s="25"/>
+      <c r="AA145" s="25"/>
+      <c r="AB145" s="25"/>
+      <c r="AC145" s="25"/>
+      <c r="AD145" s="25"/>
+      <c r="AE145" s="25"/>
+      <c r="AF145" s="25"/>
+      <c r="AG145" s="25"/>
+      <c r="AH145" s="25"/>
+      <c r="AI145" s="25"/>
+    </row>
+    <row r="146" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A146" s="25"/>
+      <c r="B146" s="66"/>
+      <c r="C146" s="66"/>
+      <c r="D146" s="25"/>
+      <c r="E146" s="25"/>
+      <c r="F146" s="25"/>
+      <c r="G146" s="25"/>
+      <c r="H146" s="25"/>
+      <c r="I146" s="25"/>
+      <c r="J146" s="25"/>
+      <c r="K146" s="25"/>
+      <c r="L146" s="25"/>
+      <c r="M146" s="25"/>
+      <c r="N146" s="25"/>
+      <c r="O146" s="25"/>
+      <c r="P146" s="25"/>
+      <c r="Q146" s="25"/>
+      <c r="R146" s="25"/>
+      <c r="S146" s="25"/>
+      <c r="T146" s="25"/>
+      <c r="U146" s="25"/>
+      <c r="V146" s="25"/>
+      <c r="W146" s="25"/>
+      <c r="X146" s="25"/>
+      <c r="Y146" s="25"/>
+      <c r="Z146" s="25"/>
+      <c r="AA146" s="25"/>
+      <c r="AB146" s="25"/>
+      <c r="AC146" s="25"/>
+      <c r="AD146" s="25"/>
+      <c r="AE146" s="25"/>
+      <c r="AF146" s="25"/>
+      <c r="AG146" s="25"/>
+      <c r="AH146" s="25"/>
+      <c r="AI146" s="25"/>
+    </row>
+    <row r="147" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A147" s="25"/>
+      <c r="B147" s="66"/>
+      <c r="C147" s="66"/>
+      <c r="D147" s="25"/>
+      <c r="E147" s="25"/>
+      <c r="F147" s="25"/>
+      <c r="G147" s="25"/>
+      <c r="H147" s="25"/>
+      <c r="I147" s="25"/>
+      <c r="J147" s="25"/>
+      <c r="K147" s="25"/>
+      <c r="L147" s="25"/>
+      <c r="M147" s="25"/>
+      <c r="N147" s="25"/>
+      <c r="O147" s="25"/>
+      <c r="P147" s="25"/>
+      <c r="Q147" s="25"/>
+      <c r="R147" s="25"/>
+      <c r="S147" s="25"/>
+      <c r="T147" s="25"/>
+      <c r="U147" s="25"/>
+      <c r="V147" s="25"/>
+      <c r="W147" s="25"/>
+      <c r="X147" s="25"/>
+      <c r="Y147" s="25"/>
+      <c r="Z147" s="25"/>
+      <c r="AA147" s="25"/>
+      <c r="AB147" s="25"/>
+      <c r="AC147" s="25"/>
+      <c r="AD147" s="25"/>
+      <c r="AE147" s="25"/>
+      <c r="AF147" s="25"/>
+      <c r="AG147" s="25"/>
+      <c r="AH147" s="25"/>
+      <c r="AI147" s="25"/>
+    </row>
+    <row r="148" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A148" s="25"/>
+      <c r="B148" s="66"/>
+      <c r="C148" s="66"/>
+      <c r="D148" s="25"/>
+      <c r="E148" s="25"/>
+      <c r="F148" s="25"/>
+      <c r="G148" s="25"/>
+      <c r="H148" s="25"/>
+      <c r="I148" s="25"/>
+      <c r="J148" s="25"/>
+      <c r="K148" s="25"/>
+      <c r="L148" s="25"/>
+      <c r="M148" s="25"/>
+      <c r="N148" s="25"/>
+      <c r="O148" s="25"/>
+      <c r="P148" s="25"/>
+      <c r="Q148" s="25"/>
+      <c r="R148" s="25"/>
+      <c r="S148" s="25"/>
+      <c r="T148" s="25"/>
+      <c r="U148" s="25"/>
+      <c r="V148" s="25"/>
+      <c r="W148" s="25"/>
+      <c r="X148" s="25"/>
+      <c r="Y148" s="25"/>
+      <c r="Z148" s="25"/>
+      <c r="AA148" s="25"/>
+      <c r="AB148" s="25"/>
+      <c r="AC148" s="25"/>
+      <c r="AD148" s="25"/>
+      <c r="AE148" s="25"/>
+      <c r="AF148" s="25"/>
+      <c r="AG148" s="25"/>
+      <c r="AH148" s="25"/>
+      <c r="AI148" s="25"/>
+    </row>
+    <row r="149" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A149" s="25"/>
+      <c r="B149" s="66"/>
+      <c r="C149" s="66"/>
+      <c r="D149" s="25"/>
+      <c r="E149" s="25"/>
+      <c r="F149" s="25"/>
+      <c r="G149" s="25"/>
+      <c r="H149" s="25"/>
+      <c r="I149" s="25"/>
+      <c r="J149" s="25"/>
+      <c r="K149" s="25"/>
+      <c r="L149" s="25"/>
+      <c r="M149" s="25"/>
+      <c r="N149" s="25"/>
+      <c r="O149" s="25"/>
+      <c r="P149" s="25"/>
+      <c r="Q149" s="25"/>
+      <c r="R149" s="25"/>
+      <c r="S149" s="25"/>
+      <c r="T149" s="25"/>
+      <c r="U149" s="25"/>
+      <c r="V149" s="25"/>
+      <c r="W149" s="25"/>
+      <c r="X149" s="25"/>
+      <c r="Y149" s="25"/>
+      <c r="Z149" s="25"/>
+      <c r="AA149" s="25"/>
+      <c r="AB149" s="25"/>
+      <c r="AC149" s="25"/>
+      <c r="AD149" s="25"/>
+      <c r="AE149" s="25"/>
+      <c r="AF149" s="25"/>
+      <c r="AG149" s="25"/>
+      <c r="AH149" s="25"/>
+      <c r="AI149" s="25"/>
+    </row>
+    <row r="150" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A150" s="25"/>
+      <c r="B150" s="66"/>
+      <c r="C150" s="66"/>
+      <c r="D150" s="25"/>
+      <c r="E150" s="25"/>
+      <c r="F150" s="25"/>
+      <c r="G150" s="25"/>
+      <c r="H150" s="25"/>
+      <c r="I150" s="25"/>
+      <c r="J150" s="25"/>
+      <c r="K150" s="25"/>
+      <c r="L150" s="25"/>
+      <c r="M150" s="25"/>
+      <c r="N150" s="25"/>
+      <c r="O150" s="25"/>
+      <c r="P150" s="25"/>
+      <c r="Q150" s="25"/>
+      <c r="R150" s="25"/>
+      <c r="S150" s="25"/>
+      <c r="T150" s="25"/>
+      <c r="U150" s="25"/>
+      <c r="V150" s="25"/>
+      <c r="W150" s="25"/>
+      <c r="X150" s="25"/>
+      <c r="Y150" s="25"/>
+      <c r="Z150" s="25"/>
+      <c r="AA150" s="25"/>
+      <c r="AB150" s="25"/>
+      <c r="AC150" s="25"/>
+      <c r="AD150" s="25"/>
+      <c r="AE150" s="25"/>
+      <c r="AF150" s="25"/>
+      <c r="AG150" s="25"/>
+      <c r="AH150" s="25"/>
+      <c r="AI150" s="25"/>
+    </row>
+    <row r="151" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A151" s="25"/>
+      <c r="B151" s="66"/>
+      <c r="C151" s="66"/>
+      <c r="D151" s="25"/>
+      <c r="E151" s="25"/>
+      <c r="F151" s="25"/>
+      <c r="G151" s="25"/>
+      <c r="H151" s="25"/>
+      <c r="I151" s="25"/>
+      <c r="J151" s="25"/>
+      <c r="K151" s="25"/>
+      <c r="L151" s="25"/>
+      <c r="M151" s="25"/>
+      <c r="N151" s="25"/>
+      <c r="O151" s="25"/>
+      <c r="P151" s="25"/>
+      <c r="Q151" s="25"/>
+      <c r="R151" s="25"/>
+      <c r="S151" s="25"/>
+      <c r="T151" s="25"/>
+      <c r="U151" s="25"/>
+      <c r="V151" s="25"/>
+      <c r="W151" s="25"/>
+      <c r="X151" s="25"/>
+      <c r="Y151" s="25"/>
+      <c r="Z151" s="25"/>
+      <c r="AA151" s="25"/>
+      <c r="AB151" s="25"/>
+      <c r="AC151" s="25"/>
+      <c r="AD151" s="25"/>
+      <c r="AE151" s="25"/>
+      <c r="AF151" s="25"/>
+      <c r="AG151" s="25"/>
+      <c r="AH151" s="25"/>
+      <c r="AI151" s="25"/>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="14">
+    <mergeCell ref="A115:AJ115"/>
+    <mergeCell ref="A125:AJ125"/>
     <mergeCell ref="C6:C8"/>
     <mergeCell ref="C10:C13"/>
     <mergeCell ref="C106:C110"/>

</xml_diff>

<commit_message>
[UPDATE] - Montly report wastu barber shop
</commit_message>
<xml_diff>
--- a/resources/template/WASTU.xlsx
+++ b/resources/template/WASTU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\hallohcga\resources\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D0034F-2AAE-40F1-8BB4-A22F7A026888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D56CE5-619F-468E-A1E2-09588AADAE2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14220" yWindow="-16560" windowWidth="29010" windowHeight="15945" xr2:uid="{96DAB095-C63E-43E2-9BFC-56E2EB8E01C9}"/>
+    <workbookView xWindow="5250" yWindow="-13515" windowWidth="21600" windowHeight="11295" xr2:uid="{96DAB095-C63E-43E2-9BFC-56E2EB8E01C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Reguler" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="113">
   <si>
     <t>Prod PIT 2</t>
   </si>
@@ -374,6 +374,9 @@
   </si>
   <si>
     <t>Magang</t>
+  </si>
+  <si>
+    <t>BARBER SHOP</t>
   </si>
 </sst>
 </file>
@@ -1225,10 +1228,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{727E0051-6F26-4AB8-8E1A-F7C7AFECA816}">
-  <dimension ref="A1:AK152"/>
+  <dimension ref="A1:AK154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="R86" sqref="R86"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="D113" sqref="A113:XFD113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1602,7 +1605,7 @@
       <c r="AH7" s="39"/>
       <c r="AI7" s="39"/>
       <c r="AJ7" s="20">
-        <f t="shared" ref="AJ7:AJ73" si="0">SUM(E7:AI7)</f>
+        <f t="shared" ref="AJ7:AJ74" si="0">SUM(E7:AI7)</f>
         <v>0</v>
       </c>
     </row>
@@ -3208,7 +3211,7 @@
       <c r="B45" s="58"/>
       <c r="C45" s="69"/>
       <c r="D45" s="17" t="s">
-        <v>46</v>
+        <v>112</v>
       </c>
       <c r="E45" s="39"/>
       <c r="F45" s="39"/>
@@ -3241,17 +3244,14 @@
       <c r="AG45" s="39"/>
       <c r="AH45" s="39"/>
       <c r="AI45" s="39"/>
-      <c r="AJ45" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="AJ45" s="20"/>
     </row>
     <row r="46" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A46" s="60"/>
       <c r="B46" s="58"/>
       <c r="C46" s="69"/>
       <c r="D46" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E46" s="39"/>
       <c r="F46" s="39"/>
@@ -3294,7 +3294,7 @@
       <c r="B47" s="58"/>
       <c r="C47" s="69"/>
       <c r="D47" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E47" s="39"/>
       <c r="F47" s="39"/>
@@ -3337,7 +3337,7 @@
       <c r="B48" s="58"/>
       <c r="C48" s="69"/>
       <c r="D48" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E48" s="39"/>
       <c r="F48" s="39"/>
@@ -3380,7 +3380,7 @@
       <c r="B49" s="58"/>
       <c r="C49" s="69"/>
       <c r="D49" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E49" s="39"/>
       <c r="F49" s="39"/>
@@ -3423,7 +3423,7 @@
       <c r="B50" s="58"/>
       <c r="C50" s="69"/>
       <c r="D50" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E50" s="39"/>
       <c r="F50" s="39"/>
@@ -3464,11 +3464,9 @@
     <row r="51" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A51" s="60"/>
       <c r="B51" s="58"/>
-      <c r="C51" s="70" t="s">
-        <v>52</v>
-      </c>
-      <c r="D51" s="16" t="s">
-        <v>53</v>
+      <c r="C51" s="69"/>
+      <c r="D51" s="17" t="s">
+        <v>51</v>
       </c>
       <c r="E51" s="39"/>
       <c r="F51" s="39"/>
@@ -3509,9 +3507,11 @@
     <row r="52" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A52" s="60"/>
       <c r="B52" s="58"/>
-      <c r="C52" s="70"/>
+      <c r="C52" s="70" t="s">
+        <v>52</v>
+      </c>
       <c r="D52" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E52" s="39"/>
       <c r="F52" s="39"/>
@@ -3554,7 +3554,7 @@
       <c r="B53" s="58"/>
       <c r="C53" s="70"/>
       <c r="D53" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E53" s="39"/>
       <c r="F53" s="39"/>
@@ -3597,7 +3597,7 @@
       <c r="B54" s="58"/>
       <c r="C54" s="70"/>
       <c r="D54" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E54" s="39"/>
       <c r="F54" s="39"/>
@@ -3640,7 +3640,7 @@
       <c r="B55" s="58"/>
       <c r="C55" s="70"/>
       <c r="D55" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E55" s="39"/>
       <c r="F55" s="39"/>
@@ -3683,7 +3683,7 @@
       <c r="B56" s="58"/>
       <c r="C56" s="70"/>
       <c r="D56" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E56" s="39"/>
       <c r="F56" s="39"/>
@@ -3725,8 +3725,8 @@
       <c r="A57" s="60"/>
       <c r="B57" s="58"/>
       <c r="C57" s="70"/>
-      <c r="D57" s="36" t="s">
-        <v>59</v>
+      <c r="D57" s="16" t="s">
+        <v>58</v>
       </c>
       <c r="E57" s="39"/>
       <c r="F57" s="39"/>
@@ -3759,14 +3759,17 @@
       <c r="AG57" s="39"/>
       <c r="AH57" s="39"/>
       <c r="AI57" s="39"/>
-      <c r="AJ57" s="20"/>
+      <c r="AJ57" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="58" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A58" s="60"/>
       <c r="B58" s="58"/>
       <c r="C58" s="70"/>
-      <c r="D58" s="37" t="s">
-        <v>107</v>
+      <c r="D58" s="36" t="s">
+        <v>59</v>
       </c>
       <c r="E58" s="39"/>
       <c r="F58" s="39"/>
@@ -3799,102 +3802,99 @@
       <c r="AG58" s="39"/>
       <c r="AH58" s="39"/>
       <c r="AI58" s="39"/>
-      <c r="AJ58" s="20">
+      <c r="AJ58" s="20"/>
+    </row>
+    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A59" s="60"/>
+      <c r="B59" s="58"/>
+      <c r="C59" s="70"/>
+      <c r="D59" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="E59" s="39"/>
+      <c r="F59" s="39"/>
+      <c r="G59" s="39"/>
+      <c r="H59" s="39"/>
+      <c r="I59" s="39"/>
+      <c r="J59" s="39"/>
+      <c r="K59" s="39"/>
+      <c r="L59" s="39"/>
+      <c r="M59" s="39"/>
+      <c r="N59" s="39"/>
+      <c r="O59" s="39"/>
+      <c r="P59" s="39"/>
+      <c r="Q59" s="39"/>
+      <c r="R59" s="39"/>
+      <c r="S59" s="39"/>
+      <c r="T59" s="39"/>
+      <c r="U59" s="39"/>
+      <c r="V59" s="39"/>
+      <c r="W59" s="39"/>
+      <c r="X59" s="39"/>
+      <c r="Y59" s="39"/>
+      <c r="Z59" s="39"/>
+      <c r="AA59" s="39"/>
+      <c r="AB59" s="39"/>
+      <c r="AC59" s="39"/>
+      <c r="AD59" s="39"/>
+      <c r="AE59" s="39"/>
+      <c r="AF59" s="39"/>
+      <c r="AG59" s="39"/>
+      <c r="AH59" s="39"/>
+      <c r="AI59" s="39"/>
+      <c r="AJ59" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:36" ht="21" x14ac:dyDescent="0.35">
-      <c r="A59" s="60"/>
-      <c r="B59" s="58"/>
-      <c r="C59" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="D59" s="33"/>
-      <c r="E59" s="33"/>
-      <c r="F59" s="33"/>
-      <c r="G59" s="33"/>
-      <c r="H59" s="33"/>
-      <c r="I59" s="33"/>
-      <c r="J59" s="33"/>
-      <c r="K59" s="33"/>
-      <c r="L59" s="33"/>
-      <c r="M59" s="33"/>
-      <c r="N59" s="33"/>
-      <c r="O59" s="33"/>
-      <c r="P59" s="33"/>
-      <c r="Q59" s="33"/>
-      <c r="R59" s="33"/>
-      <c r="S59" s="33"/>
-      <c r="T59" s="33"/>
-      <c r="U59" s="33"/>
-      <c r="V59" s="33"/>
-      <c r="W59" s="33"/>
-      <c r="X59" s="33"/>
-      <c r="Y59" s="33"/>
-      <c r="Z59" s="33"/>
-      <c r="AA59" s="33"/>
-      <c r="AB59" s="33"/>
-      <c r="AC59" s="33"/>
-      <c r="AD59" s="33"/>
-      <c r="AE59" s="33"/>
-      <c r="AF59" s="33"/>
-      <c r="AG59" s="33"/>
-      <c r="AH59" s="33"/>
-      <c r="AI59" s="34"/>
-      <c r="AJ59" s="20"/>
-    </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:36" ht="21" x14ac:dyDescent="0.35">
       <c r="A60" s="60"/>
       <c r="B60" s="58"/>
-      <c r="C60" s="61" t="s">
+      <c r="C60" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="D60" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="E60" s="39"/>
-      <c r="F60" s="39"/>
-      <c r="G60" s="39"/>
-      <c r="H60" s="39"/>
-      <c r="I60" s="39"/>
-      <c r="J60" s="39"/>
-      <c r="K60" s="39"/>
-      <c r="L60" s="39"/>
-      <c r="M60" s="39"/>
-      <c r="N60" s="39"/>
-      <c r="O60" s="39"/>
-      <c r="P60" s="39"/>
-      <c r="Q60" s="39"/>
-      <c r="R60" s="39"/>
-      <c r="S60" s="39"/>
-      <c r="T60" s="39"/>
-      <c r="U60" s="39"/>
-      <c r="V60" s="39"/>
-      <c r="W60" s="39"/>
-      <c r="X60" s="39"/>
-      <c r="Y60" s="39"/>
-      <c r="Z60" s="39"/>
-      <c r="AA60" s="39"/>
-      <c r="AB60" s="39"/>
-      <c r="AC60" s="39"/>
-      <c r="AD60" s="39"/>
-      <c r="AE60" s="39"/>
-      <c r="AF60" s="39"/>
-      <c r="AG60" s="39"/>
-      <c r="AH60" s="39"/>
-      <c r="AI60" s="39"/>
-      <c r="AJ60" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D60" s="33"/>
+      <c r="E60" s="33"/>
+      <c r="F60" s="33"/>
+      <c r="G60" s="33"/>
+      <c r="H60" s="33"/>
+      <c r="I60" s="33"/>
+      <c r="J60" s="33"/>
+      <c r="K60" s="33"/>
+      <c r="L60" s="33"/>
+      <c r="M60" s="33"/>
+      <c r="N60" s="33"/>
+      <c r="O60" s="33"/>
+      <c r="P60" s="33"/>
+      <c r="Q60" s="33"/>
+      <c r="R60" s="33"/>
+      <c r="S60" s="33"/>
+      <c r="T60" s="33"/>
+      <c r="U60" s="33"/>
+      <c r="V60" s="33"/>
+      <c r="W60" s="33"/>
+      <c r="X60" s="33"/>
+      <c r="Y60" s="33"/>
+      <c r="Z60" s="33"/>
+      <c r="AA60" s="33"/>
+      <c r="AB60" s="33"/>
+      <c r="AC60" s="33"/>
+      <c r="AD60" s="33"/>
+      <c r="AE60" s="33"/>
+      <c r="AF60" s="33"/>
+      <c r="AG60" s="33"/>
+      <c r="AH60" s="33"/>
+      <c r="AI60" s="34"/>
+      <c r="AJ60" s="20"/>
     </row>
     <row r="61" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A61" s="60"/>
       <c r="B61" s="58"/>
-      <c r="C61" s="62"/>
+      <c r="C61" s="61" t="s">
+        <v>60</v>
+      </c>
       <c r="D61" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E61" s="39"/>
       <c r="F61" s="39"/>
@@ -3937,7 +3937,7 @@
       <c r="B62" s="58"/>
       <c r="C62" s="62"/>
       <c r="D62" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E62" s="39"/>
       <c r="F62" s="39"/>
@@ -3980,7 +3980,7 @@
       <c r="B63" s="58"/>
       <c r="C63" s="62"/>
       <c r="D63" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E63" s="39"/>
       <c r="F63" s="39"/>
@@ -4023,7 +4023,7 @@
       <c r="B64" s="58"/>
       <c r="C64" s="62"/>
       <c r="D64" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E64" s="39"/>
       <c r="F64" s="39"/>
@@ -4066,7 +4066,7 @@
       <c r="B65" s="58"/>
       <c r="C65" s="62"/>
       <c r="D65" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E65" s="39"/>
       <c r="F65" s="39"/>
@@ -4109,7 +4109,7 @@
       <c r="B66" s="58"/>
       <c r="C66" s="62"/>
       <c r="D66" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E66" s="39"/>
       <c r="F66" s="39"/>
@@ -4152,7 +4152,7 @@
       <c r="B67" s="58"/>
       <c r="C67" s="62"/>
       <c r="D67" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E67" s="39"/>
       <c r="F67" s="39"/>
@@ -4195,7 +4195,7 @@
       <c r="B68" s="58"/>
       <c r="C68" s="62"/>
       <c r="D68" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E68" s="39"/>
       <c r="F68" s="39"/>
@@ -4238,7 +4238,7 @@
       <c r="B69" s="58"/>
       <c r="C69" s="62"/>
       <c r="D69" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E69" s="39"/>
       <c r="F69" s="39"/>
@@ -4281,7 +4281,7 @@
       <c r="B70" s="58"/>
       <c r="C70" s="62"/>
       <c r="D70" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E70" s="39"/>
       <c r="F70" s="39"/>
@@ -4324,7 +4324,7 @@
       <c r="B71" s="58"/>
       <c r="C71" s="62"/>
       <c r="D71" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E71" s="39"/>
       <c r="F71" s="39"/>
@@ -4367,7 +4367,7 @@
       <c r="B72" s="58"/>
       <c r="C72" s="62"/>
       <c r="D72" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E72" s="39"/>
       <c r="F72" s="39"/>
@@ -4408,9 +4408,9 @@
     <row r="73" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A73" s="60"/>
       <c r="B73" s="58"/>
-      <c r="C73" s="63"/>
+      <c r="C73" s="62"/>
       <c r="D73" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E73" s="39"/>
       <c r="F73" s="39"/>
@@ -4448,14 +4448,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A74" s="60"/>
       <c r="B74" s="58"/>
-      <c r="C74" s="12" t="s">
-        <v>101</v>
-      </c>
+      <c r="C74" s="63"/>
       <c r="D74" s="11" t="s">
-        <v>7</v>
+        <v>74</v>
       </c>
       <c r="E74" s="39"/>
       <c r="F74" s="39"/>
@@ -4489,101 +4487,103 @@
       <c r="AH74" s="39"/>
       <c r="AI74" s="39"/>
       <c r="AJ74" s="20">
-        <f t="shared" ref="AJ74:AJ111" si="1">SUM(E74:AI74)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:36" ht="21" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="60"/>
       <c r="B75" s="58"/>
-      <c r="C75" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="D75" s="33"/>
-      <c r="E75" s="33"/>
-      <c r="F75" s="33"/>
-      <c r="G75" s="33"/>
-      <c r="H75" s="33"/>
-      <c r="I75" s="33"/>
-      <c r="J75" s="33"/>
-      <c r="K75" s="33"/>
-      <c r="L75" s="33"/>
-      <c r="M75" s="33"/>
-      <c r="N75" s="33"/>
-      <c r="O75" s="33"/>
-      <c r="P75" s="33"/>
-      <c r="Q75" s="33"/>
-      <c r="R75" s="33"/>
-      <c r="S75" s="33"/>
-      <c r="T75" s="33"/>
-      <c r="U75" s="33"/>
-      <c r="V75" s="33"/>
-      <c r="W75" s="33"/>
-      <c r="X75" s="33"/>
-      <c r="Y75" s="33"/>
-      <c r="Z75" s="33"/>
-      <c r="AA75" s="33"/>
-      <c r="AB75" s="33"/>
-      <c r="AC75" s="33"/>
-      <c r="AD75" s="33"/>
-      <c r="AE75" s="33"/>
-      <c r="AF75" s="33"/>
-      <c r="AG75" s="33"/>
-      <c r="AH75" s="33"/>
-      <c r="AI75" s="34"/>
-      <c r="AJ75" s="20"/>
-    </row>
-    <row r="76" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C75" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D75" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E75" s="39"/>
+      <c r="F75" s="39"/>
+      <c r="G75" s="39"/>
+      <c r="H75" s="39"/>
+      <c r="I75" s="39"/>
+      <c r="J75" s="39"/>
+      <c r="K75" s="39"/>
+      <c r="L75" s="39"/>
+      <c r="M75" s="39"/>
+      <c r="N75" s="39"/>
+      <c r="O75" s="39"/>
+      <c r="P75" s="39"/>
+      <c r="Q75" s="39"/>
+      <c r="R75" s="39"/>
+      <c r="S75" s="39"/>
+      <c r="T75" s="39"/>
+      <c r="U75" s="39"/>
+      <c r="V75" s="39"/>
+      <c r="W75" s="39"/>
+      <c r="X75" s="39"/>
+      <c r="Y75" s="39"/>
+      <c r="Z75" s="39"/>
+      <c r="AA75" s="39"/>
+      <c r="AB75" s="39"/>
+      <c r="AC75" s="39"/>
+      <c r="AD75" s="39"/>
+      <c r="AE75" s="39"/>
+      <c r="AF75" s="39"/>
+      <c r="AG75" s="39"/>
+      <c r="AH75" s="39"/>
+      <c r="AI75" s="39"/>
+      <c r="AJ75" s="20">
+        <f t="shared" ref="AJ75:AJ113" si="1">SUM(E75:AI75)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:36" ht="21" x14ac:dyDescent="0.35">
       <c r="A76" s="60"/>
       <c r="B76" s="58"/>
-      <c r="C76" s="64" t="s">
+      <c r="C76" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="D76" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="E76" s="39"/>
-      <c r="F76" s="39"/>
-      <c r="G76" s="39"/>
-      <c r="H76" s="39"/>
-      <c r="I76" s="39"/>
-      <c r="J76" s="39"/>
-      <c r="K76" s="39"/>
-      <c r="L76" s="39"/>
-      <c r="M76" s="39"/>
-      <c r="N76" s="39"/>
-      <c r="O76" s="39"/>
-      <c r="P76" s="39"/>
-      <c r="Q76" s="39"/>
-      <c r="R76" s="39"/>
-      <c r="S76" s="39"/>
-      <c r="T76" s="39"/>
-      <c r="U76" s="39"/>
-      <c r="V76" s="39"/>
-      <c r="W76" s="39"/>
-      <c r="X76" s="39"/>
-      <c r="Y76" s="39"/>
-      <c r="Z76" s="39"/>
-      <c r="AA76" s="39"/>
-      <c r="AB76" s="39"/>
-      <c r="AC76" s="39"/>
-      <c r="AD76" s="39"/>
-      <c r="AE76" s="39"/>
-      <c r="AF76" s="39"/>
-      <c r="AG76" s="39"/>
-      <c r="AH76" s="39"/>
-      <c r="AI76" s="39"/>
-      <c r="AJ76" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="D76" s="33"/>
+      <c r="E76" s="33"/>
+      <c r="F76" s="33"/>
+      <c r="G76" s="33"/>
+      <c r="H76" s="33"/>
+      <c r="I76" s="33"/>
+      <c r="J76" s="33"/>
+      <c r="K76" s="33"/>
+      <c r="L76" s="33"/>
+      <c r="M76" s="33"/>
+      <c r="N76" s="33"/>
+      <c r="O76" s="33"/>
+      <c r="P76" s="33"/>
+      <c r="Q76" s="33"/>
+      <c r="R76" s="33"/>
+      <c r="S76" s="33"/>
+      <c r="T76" s="33"/>
+      <c r="U76" s="33"/>
+      <c r="V76" s="33"/>
+      <c r="W76" s="33"/>
+      <c r="X76" s="33"/>
+      <c r="Y76" s="33"/>
+      <c r="Z76" s="33"/>
+      <c r="AA76" s="33"/>
+      <c r="AB76" s="33"/>
+      <c r="AC76" s="33"/>
+      <c r="AD76" s="33"/>
+      <c r="AE76" s="33"/>
+      <c r="AF76" s="33"/>
+      <c r="AG76" s="33"/>
+      <c r="AH76" s="33"/>
+      <c r="AI76" s="34"/>
+      <c r="AJ76" s="20"/>
     </row>
     <row r="77" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="60"/>
       <c r="B77" s="58"/>
-      <c r="C77" s="65"/>
+      <c r="C77" s="64" t="s">
+        <v>75</v>
+      </c>
       <c r="D77" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E77" s="39"/>
       <c r="F77" s="39"/>
@@ -4626,7 +4626,7 @@
       <c r="B78" s="58"/>
       <c r="C78" s="65"/>
       <c r="D78" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E78" s="39"/>
       <c r="F78" s="39"/>
@@ -4669,7 +4669,7 @@
       <c r="B79" s="58"/>
       <c r="C79" s="65"/>
       <c r="D79" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E79" s="39"/>
       <c r="F79" s="39"/>
@@ -4712,7 +4712,7 @@
       <c r="B80" s="58"/>
       <c r="C80" s="65"/>
       <c r="D80" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E80" s="39"/>
       <c r="F80" s="39"/>
@@ -4750,12 +4750,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="60"/>
       <c r="B81" s="58"/>
       <c r="C81" s="65"/>
-      <c r="D81" s="14" t="s">
-        <v>81</v>
+      <c r="D81" s="13" t="s">
+        <v>80</v>
       </c>
       <c r="E81" s="39"/>
       <c r="F81" s="39"/>
@@ -4798,7 +4798,7 @@
       <c r="B82" s="58"/>
       <c r="C82" s="65"/>
       <c r="D82" s="13" t="s">
-        <v>82</v>
+        <v>112</v>
       </c>
       <c r="E82" s="39"/>
       <c r="F82" s="39"/>
@@ -4831,17 +4831,14 @@
       <c r="AG82" s="39"/>
       <c r="AH82" s="39"/>
       <c r="AI82" s="39"/>
-      <c r="AJ82" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="AJ82" s="20"/>
+    </row>
+    <row r="83" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A83" s="60"/>
       <c r="B83" s="58"/>
       <c r="C83" s="65"/>
-      <c r="D83" s="13" t="s">
-        <v>83</v>
+      <c r="D83" s="14" t="s">
+        <v>81</v>
       </c>
       <c r="E83" s="39"/>
       <c r="F83" s="39"/>
@@ -4884,7 +4881,7 @@
       <c r="B84" s="58"/>
       <c r="C84" s="65"/>
       <c r="D84" s="13" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="E84" s="39"/>
       <c r="F84" s="39"/>
@@ -4927,7 +4924,7 @@
       <c r="B85" s="58"/>
       <c r="C85" s="65"/>
       <c r="D85" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E85" s="39"/>
       <c r="F85" s="39"/>
@@ -4970,7 +4967,7 @@
       <c r="B86" s="58"/>
       <c r="C86" s="65"/>
       <c r="D86" s="13" t="s">
-        <v>85</v>
+        <v>41</v>
       </c>
       <c r="E86" s="39"/>
       <c r="F86" s="39"/>
@@ -5013,7 +5010,7 @@
       <c r="B87" s="58"/>
       <c r="C87" s="65"/>
       <c r="D87" s="13" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="E87" s="39"/>
       <c r="F87" s="39"/>
@@ -5056,7 +5053,7 @@
       <c r="B88" s="58"/>
       <c r="C88" s="65"/>
       <c r="D88" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E88" s="39"/>
       <c r="F88" s="39"/>
@@ -5099,7 +5096,7 @@
       <c r="B89" s="58"/>
       <c r="C89" s="65"/>
       <c r="D89" s="13" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="E89" s="39"/>
       <c r="F89" s="39"/>
@@ -5142,7 +5139,7 @@
       <c r="B90" s="58"/>
       <c r="C90" s="65"/>
       <c r="D90" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E90" s="39"/>
       <c r="F90" s="39"/>
@@ -5185,7 +5182,7 @@
       <c r="B91" s="58"/>
       <c r="C91" s="65"/>
       <c r="D91" s="13" t="s">
-        <v>2</v>
+        <v>87</v>
       </c>
       <c r="E91" s="39"/>
       <c r="F91" s="39"/>
@@ -5228,7 +5225,7 @@
       <c r="B92" s="58"/>
       <c r="C92" s="65"/>
       <c r="D92" s="13" t="s">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="E92" s="39"/>
       <c r="F92" s="39"/>
@@ -5271,7 +5268,7 @@
       <c r="B93" s="58"/>
       <c r="C93" s="65"/>
       <c r="D93" s="13" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E93" s="39"/>
       <c r="F93" s="39"/>
@@ -5314,7 +5311,7 @@
       <c r="B94" s="58"/>
       <c r="C94" s="65"/>
       <c r="D94" s="13" t="s">
-        <v>89</v>
+        <v>0</v>
       </c>
       <c r="E94" s="39"/>
       <c r="F94" s="39"/>
@@ -5357,7 +5354,7 @@
       <c r="B95" s="58"/>
       <c r="C95" s="65"/>
       <c r="D95" s="13" t="s">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="E95" s="39"/>
       <c r="F95" s="39"/>
@@ -5400,7 +5397,7 @@
       <c r="B96" s="58"/>
       <c r="C96" s="65"/>
       <c r="D96" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E96" s="39"/>
       <c r="F96" s="39"/>
@@ -5443,7 +5440,7 @@
       <c r="B97" s="58"/>
       <c r="C97" s="65"/>
       <c r="D97" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E97" s="39"/>
       <c r="F97" s="39"/>
@@ -5486,7 +5483,7 @@
       <c r="B98" s="58"/>
       <c r="C98" s="65"/>
       <c r="D98" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E98" s="39"/>
       <c r="F98" s="39"/>
@@ -5529,7 +5526,7 @@
       <c r="B99" s="58"/>
       <c r="C99" s="65"/>
       <c r="D99" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E99" s="39"/>
       <c r="F99" s="39"/>
@@ -5572,7 +5569,7 @@
       <c r="B100" s="58"/>
       <c r="C100" s="65"/>
       <c r="D100" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E100" s="39"/>
       <c r="F100" s="39"/>
@@ -5615,7 +5612,7 @@
       <c r="B101" s="58"/>
       <c r="C101" s="65"/>
       <c r="D101" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E101" s="39"/>
       <c r="F101" s="39"/>
@@ -5658,7 +5655,7 @@
       <c r="B102" s="58"/>
       <c r="C102" s="65"/>
       <c r="D102" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E102" s="39"/>
       <c r="F102" s="39"/>
@@ -5701,7 +5698,7 @@
       <c r="B103" s="58"/>
       <c r="C103" s="65"/>
       <c r="D103" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E103" s="39"/>
       <c r="F103" s="39"/>
@@ -5744,7 +5741,7 @@
       <c r="B104" s="58"/>
       <c r="C104" s="65"/>
       <c r="D104" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E104" s="39"/>
       <c r="F104" s="39"/>
@@ -5785,9 +5782,9 @@
     <row r="105" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="60"/>
       <c r="B105" s="58"/>
-      <c r="C105" s="66"/>
+      <c r="C105" s="65"/>
       <c r="D105" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E105" s="39"/>
       <c r="F105" s="39"/>
@@ -5825,54 +5822,55 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:36" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="60"/>
       <c r="B106" s="58"/>
-      <c r="C106" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="D106" s="26"/>
-      <c r="E106" s="26"/>
-      <c r="F106" s="26"/>
-      <c r="G106" s="26"/>
-      <c r="H106" s="26"/>
-      <c r="I106" s="26"/>
-      <c r="J106" s="26"/>
-      <c r="K106" s="26"/>
-      <c r="L106" s="26"/>
-      <c r="M106" s="26"/>
-      <c r="N106" s="26"/>
-      <c r="O106" s="26"/>
-      <c r="P106" s="26"/>
-      <c r="Q106" s="26"/>
-      <c r="R106" s="26"/>
-      <c r="S106" s="26"/>
-      <c r="T106" s="26"/>
-      <c r="U106" s="26"/>
-      <c r="V106" s="26"/>
-      <c r="W106" s="26"/>
-      <c r="X106" s="26"/>
-      <c r="Y106" s="26"/>
-      <c r="Z106" s="26"/>
-      <c r="AA106" s="26"/>
-      <c r="AB106" s="26"/>
-      <c r="AC106" s="26"/>
-      <c r="AD106" s="26"/>
-      <c r="AE106" s="26"/>
-      <c r="AF106" s="26"/>
-      <c r="AG106" s="26"/>
-      <c r="AH106" s="26"/>
-      <c r="AI106" s="26"/>
-      <c r="AJ106" s="26"/>
+      <c r="C106" s="65"/>
+      <c r="D106" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E106" s="39"/>
+      <c r="F106" s="39"/>
+      <c r="G106" s="39"/>
+      <c r="H106" s="39"/>
+      <c r="I106" s="39"/>
+      <c r="J106" s="39"/>
+      <c r="K106" s="39"/>
+      <c r="L106" s="39"/>
+      <c r="M106" s="39"/>
+      <c r="N106" s="39"/>
+      <c r="O106" s="39"/>
+      <c r="P106" s="39"/>
+      <c r="Q106" s="39"/>
+      <c r="R106" s="39"/>
+      <c r="S106" s="39"/>
+      <c r="T106" s="39"/>
+      <c r="U106" s="39"/>
+      <c r="V106" s="39"/>
+      <c r="W106" s="39"/>
+      <c r="X106" s="39"/>
+      <c r="Y106" s="39"/>
+      <c r="Z106" s="39"/>
+      <c r="AA106" s="39"/>
+      <c r="AB106" s="39"/>
+      <c r="AC106" s="39"/>
+      <c r="AD106" s="39"/>
+      <c r="AE106" s="39"/>
+      <c r="AF106" s="39"/>
+      <c r="AG106" s="39"/>
+      <c r="AH106" s="39"/>
+      <c r="AI106" s="39"/>
+      <c r="AJ106" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="107" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="60"/>
       <c r="B107" s="58"/>
-      <c r="C107" s="56" t="s">
-        <v>106</v>
-      </c>
-      <c r="D107" s="24" t="s">
-        <v>103</v>
+      <c r="C107" s="66"/>
+      <c r="D107" s="13" t="s">
+        <v>100</v>
       </c>
       <c r="E107" s="39"/>
       <c r="F107" s="39"/>
@@ -5906,59 +5904,58 @@
       <c r="AH107" s="39"/>
       <c r="AI107" s="39"/>
       <c r="AJ107" s="20">
-        <f>SUM(E107:AI107)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:36" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A108" s="60"/>
       <c r="B108" s="58"/>
-      <c r="C108" s="56"/>
-      <c r="D108" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="E108" s="39"/>
-      <c r="F108" s="39"/>
-      <c r="G108" s="39"/>
-      <c r="H108" s="39"/>
-      <c r="I108" s="39"/>
-      <c r="J108" s="39"/>
-      <c r="K108" s="39"/>
-      <c r="L108" s="39"/>
-      <c r="M108" s="39"/>
-      <c r="N108" s="39"/>
-      <c r="O108" s="39"/>
-      <c r="P108" s="39"/>
-      <c r="Q108" s="39"/>
-      <c r="R108" s="39"/>
-      <c r="S108" s="39"/>
-      <c r="T108" s="39"/>
-      <c r="U108" s="39"/>
-      <c r="V108" s="39"/>
-      <c r="W108" s="39"/>
-      <c r="X108" s="39"/>
-      <c r="Y108" s="39"/>
-      <c r="Z108" s="39"/>
-      <c r="AA108" s="39"/>
-      <c r="AB108" s="39"/>
-      <c r="AC108" s="39"/>
-      <c r="AD108" s="39"/>
-      <c r="AE108" s="39"/>
-      <c r="AF108" s="39"/>
-      <c r="AG108" s="39"/>
-      <c r="AH108" s="39"/>
-      <c r="AI108" s="39"/>
-      <c r="AJ108" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="C108" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="D108" s="26"/>
+      <c r="E108" s="26"/>
+      <c r="F108" s="26"/>
+      <c r="G108" s="26"/>
+      <c r="H108" s="26"/>
+      <c r="I108" s="26"/>
+      <c r="J108" s="26"/>
+      <c r="K108" s="26"/>
+      <c r="L108" s="26"/>
+      <c r="M108" s="26"/>
+      <c r="N108" s="26"/>
+      <c r="O108" s="26"/>
+      <c r="P108" s="26"/>
+      <c r="Q108" s="26"/>
+      <c r="R108" s="26"/>
+      <c r="S108" s="26"/>
+      <c r="T108" s="26"/>
+      <c r="U108" s="26"/>
+      <c r="V108" s="26"/>
+      <c r="W108" s="26"/>
+      <c r="X108" s="26"/>
+      <c r="Y108" s="26"/>
+      <c r="Z108" s="26"/>
+      <c r="AA108" s="26"/>
+      <c r="AB108" s="26"/>
+      <c r="AC108" s="26"/>
+      <c r="AD108" s="26"/>
+      <c r="AE108" s="26"/>
+      <c r="AF108" s="26"/>
+      <c r="AG108" s="26"/>
+      <c r="AH108" s="26"/>
+      <c r="AI108" s="26"/>
+      <c r="AJ108" s="26"/>
     </row>
     <row r="109" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="60"/>
       <c r="B109" s="58"/>
-      <c r="C109" s="56"/>
+      <c r="C109" s="56" t="s">
+        <v>106</v>
+      </c>
       <c r="D109" s="24" t="s">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="E109" s="39"/>
       <c r="F109" s="39"/>
@@ -5992,7 +5989,7 @@
       <c r="AH109" s="39"/>
       <c r="AI109" s="39"/>
       <c r="AJ109" s="20">
-        <f t="shared" si="1"/>
+        <f>SUM(E109:AI109)</f>
         <v>0</v>
       </c>
     </row>
@@ -6001,7 +5998,7 @@
       <c r="B110" s="58"/>
       <c r="C110" s="56"/>
       <c r="D110" s="24" t="s">
-        <v>104</v>
+        <v>66</v>
       </c>
       <c r="E110" s="39"/>
       <c r="F110" s="39"/>
@@ -6044,7 +6041,7 @@
       <c r="B111" s="58"/>
       <c r="C111" s="56"/>
       <c r="D111" s="24" t="s">
-        <v>105</v>
+        <v>64</v>
       </c>
       <c r="E111" s="39"/>
       <c r="F111" s="39"/>
@@ -6082,362 +6079,374 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="E112" s="41">
-        <f>SUM(E3:E111)</f>
+    <row r="112" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A112" s="60"/>
+      <c r="B112" s="58"/>
+      <c r="C112" s="56"/>
+      <c r="D112" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="E112" s="39"/>
+      <c r="F112" s="39"/>
+      <c r="G112" s="39"/>
+      <c r="H112" s="39"/>
+      <c r="I112" s="39"/>
+      <c r="J112" s="39"/>
+      <c r="K112" s="39"/>
+      <c r="L112" s="39"/>
+      <c r="M112" s="39"/>
+      <c r="N112" s="39"/>
+      <c r="O112" s="39"/>
+      <c r="P112" s="39"/>
+      <c r="Q112" s="39"/>
+      <c r="R112" s="39"/>
+      <c r="S112" s="39"/>
+      <c r="T112" s="39"/>
+      <c r="U112" s="39"/>
+      <c r="V112" s="39"/>
+      <c r="W112" s="39"/>
+      <c r="X112" s="39"/>
+      <c r="Y112" s="39"/>
+      <c r="Z112" s="39"/>
+      <c r="AA112" s="39"/>
+      <c r="AB112" s="39"/>
+      <c r="AC112" s="39"/>
+      <c r="AD112" s="39"/>
+      <c r="AE112" s="39"/>
+      <c r="AF112" s="39"/>
+      <c r="AG112" s="39"/>
+      <c r="AH112" s="39"/>
+      <c r="AI112" s="39"/>
+      <c r="AJ112" s="20">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F112" s="41">
-        <f>SUM(F3:F111)</f>
+    </row>
+    <row r="113" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A113" s="60"/>
+      <c r="B113" s="58"/>
+      <c r="C113" s="56"/>
+      <c r="D113" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="E113" s="39"/>
+      <c r="F113" s="39"/>
+      <c r="G113" s="39"/>
+      <c r="H113" s="39"/>
+      <c r="I113" s="39"/>
+      <c r="J113" s="39"/>
+      <c r="K113" s="39"/>
+      <c r="L113" s="39"/>
+      <c r="M113" s="39"/>
+      <c r="N113" s="39"/>
+      <c r="O113" s="39"/>
+      <c r="P113" s="39"/>
+      <c r="Q113" s="39"/>
+      <c r="R113" s="39"/>
+      <c r="S113" s="39"/>
+      <c r="T113" s="39"/>
+      <c r="U113" s="39"/>
+      <c r="V113" s="39"/>
+      <c r="W113" s="39"/>
+      <c r="X113" s="39"/>
+      <c r="Y113" s="39"/>
+      <c r="Z113" s="39"/>
+      <c r="AA113" s="39"/>
+      <c r="AB113" s="39"/>
+      <c r="AC113" s="39"/>
+      <c r="AD113" s="39"/>
+      <c r="AE113" s="39"/>
+      <c r="AF113" s="39"/>
+      <c r="AG113" s="39"/>
+      <c r="AH113" s="39"/>
+      <c r="AI113" s="39"/>
+      <c r="AJ113" s="20">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G112" s="41">
-        <f t="shared" ref="G112:AI112" si="2">SUM(G3:G111)</f>
+    </row>
+    <row r="114" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="E114" s="41">
+        <f>SUM(E3:E113)</f>
         <v>0</v>
       </c>
-      <c r="H112" s="41">
+      <c r="F114" s="41">
+        <f>SUM(F3:F113)</f>
+        <v>0</v>
+      </c>
+      <c r="G114" s="41">
+        <f t="shared" ref="G114:AI114" si="2">SUM(G3:G113)</f>
+        <v>0</v>
+      </c>
+      <c r="H114" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I112" s="41">
+      <c r="I114" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J112" s="41">
+      <c r="J114" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K112" s="41">
+      <c r="K114" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L112" s="41">
+      <c r="L114" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M112" s="41">
-        <f>SUM(M3:M111)</f>
+      <c r="M114" s="41">
+        <f>SUM(M3:M113)</f>
         <v>0</v>
       </c>
-      <c r="N112" s="41">
-        <f>SUM(N3:N111)</f>
+      <c r="N114" s="41">
+        <f>SUM(N3:N113)</f>
         <v>0</v>
       </c>
-      <c r="O112" s="41">
+      <c r="O114" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P112" s="41">
+      <c r="P114" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q112" s="41">
+      <c r="Q114" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R112" s="41">
+      <c r="R114" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S112" s="41">
+      <c r="S114" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T112" s="41">
+      <c r="T114" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U112" s="41">
+      <c r="U114" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="V112" s="41">
+      <c r="V114" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="W112" s="41">
+      <c r="W114" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X112" s="41">
+      <c r="X114" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y112" s="41">
+      <c r="Y114" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Z112" s="41">
+      <c r="Z114" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA112" s="41">
+      <c r="AA114" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB112" s="41">
+      <c r="AB114" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC112" s="41">
+      <c r="AC114" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AD112" s="41">
+      <c r="AD114" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AE112" s="41">
+      <c r="AE114" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AF112" s="41">
+      <c r="AF114" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AG112" s="41">
+      <c r="AG114" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AH112" s="41">
+      <c r="AH114" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AI112" s="41">
+      <c r="AI114" s="41">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="AI114" s="22" t="s">
+    <row r="116" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AI116" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="AJ114" s="23">
-        <f>SUM(AJ3:AJ105)</f>
+      <c r="AJ116" s="23">
+        <f>SUM(AJ3:AJ107)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:36" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A116" s="52" t="s">
+    <row r="118" spans="1:36" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A118" s="52" t="s">
         <v>108</v>
       </c>
-      <c r="B116" s="53"/>
-      <c r="C116" s="53"/>
-      <c r="D116" s="53"/>
-      <c r="E116" s="53"/>
-      <c r="F116" s="53"/>
-      <c r="G116" s="53"/>
-      <c r="H116" s="53"/>
-      <c r="I116" s="53"/>
-      <c r="J116" s="53"/>
-      <c r="K116" s="53"/>
-      <c r="L116" s="53"/>
-      <c r="M116" s="53"/>
-      <c r="N116" s="53"/>
-      <c r="O116" s="53"/>
-      <c r="P116" s="53"/>
-      <c r="Q116" s="53"/>
-      <c r="R116" s="53"/>
-      <c r="S116" s="53"/>
-      <c r="T116" s="53"/>
-      <c r="U116" s="53"/>
-      <c r="V116" s="53"/>
-      <c r="W116" s="53"/>
-      <c r="X116" s="53"/>
-      <c r="Y116" s="53"/>
-      <c r="Z116" s="53"/>
-      <c r="AA116" s="53"/>
-      <c r="AB116" s="53"/>
-      <c r="AC116" s="53"/>
-      <c r="AD116" s="53"/>
-      <c r="AE116" s="53"/>
-      <c r="AF116" s="53"/>
-      <c r="AG116" s="53"/>
-      <c r="AH116" s="53"/>
-      <c r="AI116" s="53"/>
-      <c r="AJ116" s="53"/>
-    </row>
-    <row r="117" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A117" s="46"/>
-      <c r="B117" s="42" t="s">
+      <c r="B118" s="53"/>
+      <c r="C118" s="53"/>
+      <c r="D118" s="53"/>
+      <c r="E118" s="53"/>
+      <c r="F118" s="53"/>
+      <c r="G118" s="53"/>
+      <c r="H118" s="53"/>
+      <c r="I118" s="53"/>
+      <c r="J118" s="53"/>
+      <c r="K118" s="53"/>
+      <c r="L118" s="53"/>
+      <c r="M118" s="53"/>
+      <c r="N118" s="53"/>
+      <c r="O118" s="53"/>
+      <c r="P118" s="53"/>
+      <c r="Q118" s="53"/>
+      <c r="R118" s="53"/>
+      <c r="S118" s="53"/>
+      <c r="T118" s="53"/>
+      <c r="U118" s="53"/>
+      <c r="V118" s="53"/>
+      <c r="W118" s="53"/>
+      <c r="X118" s="53"/>
+      <c r="Y118" s="53"/>
+      <c r="Z118" s="53"/>
+      <c r="AA118" s="53"/>
+      <c r="AB118" s="53"/>
+      <c r="AC118" s="53"/>
+      <c r="AD118" s="53"/>
+      <c r="AE118" s="53"/>
+      <c r="AF118" s="53"/>
+      <c r="AG118" s="53"/>
+      <c r="AH118" s="53"/>
+      <c r="AI118" s="53"/>
+      <c r="AJ118" s="53"/>
+    </row>
+    <row r="119" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A119" s="46"/>
+      <c r="B119" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="C117" s="43" t="s">
+      <c r="C119" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="D117" s="43" t="s">
+      <c r="D119" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="E117" s="15">
+      <c r="E119" s="15">
         <v>1</v>
       </c>
-      <c r="F117" s="15">
+      <c r="F119" s="15">
         <v>2</v>
       </c>
-      <c r="G117" s="15">
+      <c r="G119" s="15">
         <v>3</v>
       </c>
-      <c r="H117" s="15">
+      <c r="H119" s="15">
         <v>4</v>
       </c>
-      <c r="I117" s="15">
+      <c r="I119" s="15">
         <v>5</v>
       </c>
-      <c r="J117" s="15">
+      <c r="J119" s="15">
         <v>6</v>
       </c>
-      <c r="K117" s="15">
+      <c r="K119" s="15">
         <v>7</v>
       </c>
-      <c r="L117" s="15">
+      <c r="L119" s="15">
         <v>8</v>
       </c>
-      <c r="M117" s="15">
+      <c r="M119" s="15">
         <v>9</v>
       </c>
-      <c r="N117" s="15">
+      <c r="N119" s="15">
         <v>10</v>
       </c>
-      <c r="O117" s="15">
+      <c r="O119" s="15">
         <v>11</v>
       </c>
-      <c r="P117" s="15">
+      <c r="P119" s="15">
         <v>12</v>
       </c>
-      <c r="Q117" s="15">
+      <c r="Q119" s="15">
         <v>13</v>
       </c>
-      <c r="R117" s="15">
+      <c r="R119" s="15">
         <v>14</v>
       </c>
-      <c r="S117" s="15">
+      <c r="S119" s="15">
         <v>15</v>
       </c>
-      <c r="T117" s="15">
+      <c r="T119" s="15">
         <v>16</v>
       </c>
-      <c r="U117" s="15">
+      <c r="U119" s="15">
         <v>17</v>
       </c>
-      <c r="V117" s="15">
+      <c r="V119" s="15">
         <v>18</v>
       </c>
-      <c r="W117" s="15">
+      <c r="W119" s="15">
         <v>19</v>
       </c>
-      <c r="X117" s="15">
+      <c r="X119" s="15">
         <v>20</v>
       </c>
-      <c r="Y117" s="15">
+      <c r="Y119" s="15">
         <v>21</v>
       </c>
-      <c r="Z117" s="15">
+      <c r="Z119" s="15">
         <v>22</v>
       </c>
-      <c r="AA117" s="15">
+      <c r="AA119" s="15">
         <v>23</v>
       </c>
-      <c r="AB117" s="15">
+      <c r="AB119" s="15">
         <v>24</v>
       </c>
-      <c r="AC117" s="15">
+      <c r="AC119" s="15">
         <v>25</v>
       </c>
-      <c r="AD117" s="15">
+      <c r="AD119" s="15">
         <v>26</v>
       </c>
-      <c r="AE117" s="15">
+      <c r="AE119" s="15">
         <v>27</v>
       </c>
-      <c r="AF117" s="15">
+      <c r="AF119" s="15">
         <v>28</v>
       </c>
-      <c r="AG117" s="15">
+      <c r="AG119" s="15">
         <v>29</v>
       </c>
-      <c r="AH117" s="15">
+      <c r="AH119" s="15">
         <v>30</v>
       </c>
-      <c r="AI117" s="15">
+      <c r="AI119" s="15">
         <v>31</v>
       </c>
-      <c r="AJ117" s="18" t="s">
+      <c r="AJ119" s="18" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="118" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A118" s="21"/>
-      <c r="B118" s="44"/>
-      <c r="C118" s="44"/>
-      <c r="D118" s="21"/>
-      <c r="E118" s="21"/>
-      <c r="F118" s="21"/>
-      <c r="G118" s="21"/>
-      <c r="H118" s="21"/>
-      <c r="I118" s="21"/>
-      <c r="J118" s="21"/>
-      <c r="K118" s="21"/>
-      <c r="L118" s="21"/>
-      <c r="M118" s="21"/>
-      <c r="N118" s="21"/>
-      <c r="O118" s="21"/>
-      <c r="P118" s="21"/>
-      <c r="Q118" s="21"/>
-      <c r="R118" s="21"/>
-      <c r="S118" s="21"/>
-      <c r="T118" s="21"/>
-      <c r="U118" s="21"/>
-      <c r="V118" s="21"/>
-      <c r="W118" s="21"/>
-      <c r="X118" s="21"/>
-      <c r="Y118" s="21"/>
-      <c r="Z118" s="21"/>
-      <c r="AA118" s="21"/>
-      <c r="AB118" s="21"/>
-      <c r="AC118" s="21"/>
-      <c r="AD118" s="21"/>
-      <c r="AE118" s="21"/>
-      <c r="AF118" s="21"/>
-      <c r="AG118" s="21"/>
-      <c r="AH118" s="21"/>
-      <c r="AI118" s="21"/>
-    </row>
-    <row r="119" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A119" s="21"/>
-      <c r="B119" s="44"/>
-      <c r="C119" s="44"/>
-      <c r="D119" s="21"/>
-      <c r="E119" s="21"/>
-      <c r="F119" s="21"/>
-      <c r="G119" s="21"/>
-      <c r="H119" s="21"/>
-      <c r="I119" s="21"/>
-      <c r="J119" s="21"/>
-      <c r="K119" s="21"/>
-      <c r="L119" s="21"/>
-      <c r="M119" s="21"/>
-      <c r="N119" s="21"/>
-      <c r="O119" s="21"/>
-      <c r="P119" s="21"/>
-      <c r="Q119" s="21"/>
-      <c r="R119" s="21"/>
-      <c r="S119" s="21"/>
-      <c r="T119" s="21"/>
-      <c r="U119" s="21"/>
-      <c r="V119" s="21"/>
-      <c r="W119" s="21"/>
-      <c r="X119" s="21"/>
-      <c r="Y119" s="21"/>
-      <c r="Z119" s="21"/>
-      <c r="AA119" s="21"/>
-      <c r="AB119" s="21"/>
-      <c r="AC119" s="21"/>
-      <c r="AD119" s="21"/>
-      <c r="AE119" s="21"/>
-      <c r="AF119" s="21"/>
-      <c r="AG119" s="21"/>
-      <c r="AH119" s="21"/>
-      <c r="AI119" s="21"/>
     </row>
     <row r="120" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A120" s="21"/>
@@ -6475,7 +6484,6 @@
       <c r="AG120" s="21"/>
       <c r="AH120" s="21"/>
       <c r="AI120" s="21"/>
-      <c r="AJ120" s="44"/>
     </row>
     <row r="121" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A121" s="21"/>
@@ -6550,6 +6558,7 @@
       <c r="AG122" s="21"/>
       <c r="AH122" s="21"/>
       <c r="AI122" s="21"/>
+      <c r="AJ122" s="44"/>
     </row>
     <row r="123" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A123" s="21"/>
@@ -6662,229 +6671,229 @@
       <c r="AH125" s="21"/>
       <c r="AI125" s="21"/>
     </row>
-    <row r="126" spans="1:36" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A126" s="52" t="s">
+    <row r="126" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A126" s="21"/>
+      <c r="B126" s="44"/>
+      <c r="C126" s="44"/>
+      <c r="D126" s="21"/>
+      <c r="E126" s="21"/>
+      <c r="F126" s="21"/>
+      <c r="G126" s="21"/>
+      <c r="H126" s="21"/>
+      <c r="I126" s="21"/>
+      <c r="J126" s="21"/>
+      <c r="K126" s="21"/>
+      <c r="L126" s="21"/>
+      <c r="M126" s="21"/>
+      <c r="N126" s="21"/>
+      <c r="O126" s="21"/>
+      <c r="P126" s="21"/>
+      <c r="Q126" s="21"/>
+      <c r="R126" s="21"/>
+      <c r="S126" s="21"/>
+      <c r="T126" s="21"/>
+      <c r="U126" s="21"/>
+      <c r="V126" s="21"/>
+      <c r="W126" s="21"/>
+      <c r="X126" s="21"/>
+      <c r="Y126" s="21"/>
+      <c r="Z126" s="21"/>
+      <c r="AA126" s="21"/>
+      <c r="AB126" s="21"/>
+      <c r="AC126" s="21"/>
+      <c r="AD126" s="21"/>
+      <c r="AE126" s="21"/>
+      <c r="AF126" s="21"/>
+      <c r="AG126" s="21"/>
+      <c r="AH126" s="21"/>
+      <c r="AI126" s="21"/>
+    </row>
+    <row r="127" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A127" s="21"/>
+      <c r="B127" s="44"/>
+      <c r="C127" s="44"/>
+      <c r="D127" s="21"/>
+      <c r="E127" s="21"/>
+      <c r="F127" s="21"/>
+      <c r="G127" s="21"/>
+      <c r="H127" s="21"/>
+      <c r="I127" s="21"/>
+      <c r="J127" s="21"/>
+      <c r="K127" s="21"/>
+      <c r="L127" s="21"/>
+      <c r="M127" s="21"/>
+      <c r="N127" s="21"/>
+      <c r="O127" s="21"/>
+      <c r="P127" s="21"/>
+      <c r="Q127" s="21"/>
+      <c r="R127" s="21"/>
+      <c r="S127" s="21"/>
+      <c r="T127" s="21"/>
+      <c r="U127" s="21"/>
+      <c r="V127" s="21"/>
+      <c r="W127" s="21"/>
+      <c r="X127" s="21"/>
+      <c r="Y127" s="21"/>
+      <c r="Z127" s="21"/>
+      <c r="AA127" s="21"/>
+      <c r="AB127" s="21"/>
+      <c r="AC127" s="21"/>
+      <c r="AD127" s="21"/>
+      <c r="AE127" s="21"/>
+      <c r="AF127" s="21"/>
+      <c r="AG127" s="21"/>
+      <c r="AH127" s="21"/>
+      <c r="AI127" s="21"/>
+    </row>
+    <row r="128" spans="1:36" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A128" s="52" t="s">
         <v>110</v>
       </c>
-      <c r="B126" s="53"/>
-      <c r="C126" s="53"/>
-      <c r="D126" s="53"/>
-      <c r="E126" s="53"/>
-      <c r="F126" s="53"/>
-      <c r="G126" s="53"/>
-      <c r="H126" s="53"/>
-      <c r="I126" s="53"/>
-      <c r="J126" s="53"/>
-      <c r="K126" s="53"/>
-      <c r="L126" s="53"/>
-      <c r="M126" s="53"/>
-      <c r="N126" s="53"/>
-      <c r="O126" s="53"/>
-      <c r="P126" s="53"/>
-      <c r="Q126" s="53"/>
-      <c r="R126" s="53"/>
-      <c r="S126" s="53"/>
-      <c r="T126" s="53"/>
-      <c r="U126" s="53"/>
-      <c r="V126" s="53"/>
-      <c r="W126" s="53"/>
-      <c r="X126" s="53"/>
-      <c r="Y126" s="53"/>
-      <c r="Z126" s="53"/>
-      <c r="AA126" s="53"/>
-      <c r="AB126" s="53"/>
-      <c r="AC126" s="53"/>
-      <c r="AD126" s="53"/>
-      <c r="AE126" s="53"/>
-      <c r="AF126" s="53"/>
-      <c r="AG126" s="53"/>
-      <c r="AH126" s="53"/>
-      <c r="AI126" s="53"/>
-      <c r="AJ126" s="53"/>
-    </row>
-    <row r="127" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A127" s="46"/>
-      <c r="B127" s="42" t="s">
+      <c r="B128" s="53"/>
+      <c r="C128" s="53"/>
+      <c r="D128" s="53"/>
+      <c r="E128" s="53"/>
+      <c r="F128" s="53"/>
+      <c r="G128" s="53"/>
+      <c r="H128" s="53"/>
+      <c r="I128" s="53"/>
+      <c r="J128" s="53"/>
+      <c r="K128" s="53"/>
+      <c r="L128" s="53"/>
+      <c r="M128" s="53"/>
+      <c r="N128" s="53"/>
+      <c r="O128" s="53"/>
+      <c r="P128" s="53"/>
+      <c r="Q128" s="53"/>
+      <c r="R128" s="53"/>
+      <c r="S128" s="53"/>
+      <c r="T128" s="53"/>
+      <c r="U128" s="53"/>
+      <c r="V128" s="53"/>
+      <c r="W128" s="53"/>
+      <c r="X128" s="53"/>
+      <c r="Y128" s="53"/>
+      <c r="Z128" s="53"/>
+      <c r="AA128" s="53"/>
+      <c r="AB128" s="53"/>
+      <c r="AC128" s="53"/>
+      <c r="AD128" s="53"/>
+      <c r="AE128" s="53"/>
+      <c r="AF128" s="53"/>
+      <c r="AG128" s="53"/>
+      <c r="AH128" s="53"/>
+      <c r="AI128" s="53"/>
+      <c r="AJ128" s="53"/>
+    </row>
+    <row r="129" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A129" s="46"/>
+      <c r="B129" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="C127" s="43" t="s">
+      <c r="C129" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="D127" s="43" t="s">
+      <c r="D129" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="E127" s="15">
+      <c r="E129" s="15">
         <v>1</v>
       </c>
-      <c r="F127" s="15">
+      <c r="F129" s="15">
         <v>2</v>
       </c>
-      <c r="G127" s="15">
+      <c r="G129" s="15">
         <v>3</v>
       </c>
-      <c r="H127" s="15">
+      <c r="H129" s="15">
         <v>4</v>
       </c>
-      <c r="I127" s="15">
+      <c r="I129" s="15">
         <v>5</v>
       </c>
-      <c r="J127" s="15">
+      <c r="J129" s="15">
         <v>6</v>
       </c>
-      <c r="K127" s="15">
+      <c r="K129" s="15">
         <v>7</v>
       </c>
-      <c r="L127" s="15">
+      <c r="L129" s="15">
         <v>8</v>
       </c>
-      <c r="M127" s="15">
+      <c r="M129" s="15">
         <v>9</v>
       </c>
-      <c r="N127" s="15">
+      <c r="N129" s="15">
         <v>10</v>
       </c>
-      <c r="O127" s="15">
+      <c r="O129" s="15">
         <v>11</v>
       </c>
-      <c r="P127" s="15">
+      <c r="P129" s="15">
         <v>12</v>
       </c>
-      <c r="Q127" s="15">
+      <c r="Q129" s="15">
         <v>13</v>
       </c>
-      <c r="R127" s="15">
+      <c r="R129" s="15">
         <v>14</v>
       </c>
-      <c r="S127" s="15">
+      <c r="S129" s="15">
         <v>15</v>
       </c>
-      <c r="T127" s="15">
+      <c r="T129" s="15">
         <v>16</v>
       </c>
-      <c r="U127" s="15">
+      <c r="U129" s="15">
         <v>17</v>
       </c>
-      <c r="V127" s="15">
+      <c r="V129" s="15">
         <v>18</v>
       </c>
-      <c r="W127" s="15">
+      <c r="W129" s="15">
         <v>19</v>
       </c>
-      <c r="X127" s="15">
+      <c r="X129" s="15">
         <v>20</v>
       </c>
-      <c r="Y127" s="15">
+      <c r="Y129" s="15">
         <v>21</v>
       </c>
-      <c r="Z127" s="15">
+      <c r="Z129" s="15">
         <v>22</v>
       </c>
-      <c r="AA127" s="15">
+      <c r="AA129" s="15">
         <v>23</v>
       </c>
-      <c r="AB127" s="15">
+      <c r="AB129" s="15">
         <v>24</v>
       </c>
-      <c r="AC127" s="15">
+      <c r="AC129" s="15">
         <v>25</v>
       </c>
-      <c r="AD127" s="15">
+      <c r="AD129" s="15">
         <v>26</v>
       </c>
-      <c r="AE127" s="15">
+      <c r="AE129" s="15">
         <v>27</v>
       </c>
-      <c r="AF127" s="15">
+      <c r="AF129" s="15">
         <v>28</v>
       </c>
-      <c r="AG127" s="15">
+      <c r="AG129" s="15">
         <v>29</v>
       </c>
-      <c r="AH127" s="15">
+      <c r="AH129" s="15">
         <v>30</v>
       </c>
-      <c r="AI127" s="15">
+      <c r="AI129" s="15">
         <v>31</v>
       </c>
-      <c r="AJ127" s="18" t="s">
+      <c r="AJ129" s="18" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="128" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A128" s="21"/>
-      <c r="B128" s="44"/>
-      <c r="C128" s="44"/>
-      <c r="D128" s="21"/>
-      <c r="E128" s="21"/>
-      <c r="F128" s="21"/>
-      <c r="G128" s="21"/>
-      <c r="H128" s="21"/>
-      <c r="I128" s="21"/>
-      <c r="J128" s="21"/>
-      <c r="K128" s="21"/>
-      <c r="L128" s="21"/>
-      <c r="M128" s="21"/>
-      <c r="N128" s="21"/>
-      <c r="O128" s="21"/>
-      <c r="P128" s="21"/>
-      <c r="Q128" s="21"/>
-      <c r="R128" s="21"/>
-      <c r="S128" s="21"/>
-      <c r="T128" s="21"/>
-      <c r="U128" s="21"/>
-      <c r="V128" s="21"/>
-      <c r="W128" s="21"/>
-      <c r="X128" s="21"/>
-      <c r="Y128" s="21"/>
-      <c r="Z128" s="21"/>
-      <c r="AA128" s="21"/>
-      <c r="AB128" s="21"/>
-      <c r="AC128" s="21"/>
-      <c r="AD128" s="21"/>
-      <c r="AE128" s="21"/>
-      <c r="AF128" s="21"/>
-      <c r="AG128" s="21"/>
-      <c r="AH128" s="21"/>
-      <c r="AI128" s="21"/>
-    </row>
-    <row r="129" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A129" s="21"/>
-      <c r="B129" s="44"/>
-      <c r="C129" s="44"/>
-      <c r="D129" s="21"/>
-      <c r="E129" s="21"/>
-      <c r="F129" s="21"/>
-      <c r="G129" s="21"/>
-      <c r="H129" s="21"/>
-      <c r="I129" s="21"/>
-      <c r="J129" s="21"/>
-      <c r="K129" s="21"/>
-      <c r="L129" s="21"/>
-      <c r="M129" s="21"/>
-      <c r="N129" s="21"/>
-      <c r="O129" s="21"/>
-      <c r="P129" s="21"/>
-      <c r="Q129" s="21"/>
-      <c r="R129" s="21"/>
-      <c r="S129" s="21"/>
-      <c r="T129" s="21"/>
-      <c r="U129" s="21"/>
-      <c r="V129" s="21"/>
-      <c r="W129" s="21"/>
-      <c r="X129" s="21"/>
-      <c r="Y129" s="21"/>
-      <c r="Z129" s="21"/>
-      <c r="AA129" s="21"/>
-      <c r="AB129" s="21"/>
-      <c r="AC129" s="21"/>
-      <c r="AD129" s="21"/>
-      <c r="AE129" s="21"/>
-      <c r="AF129" s="21"/>
-      <c r="AG129" s="21"/>
-      <c r="AH129" s="21"/>
-      <c r="AI129" s="21"/>
-    </row>
-    <row r="130" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A130" s="21"/>
       <c r="B130" s="44"/>
       <c r="C130" s="44"/>
@@ -6921,7 +6930,7 @@
       <c r="AH130" s="21"/>
       <c r="AI130" s="21"/>
     </row>
-    <row r="131" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A131" s="21"/>
       <c r="B131" s="44"/>
       <c r="C131" s="44"/>
@@ -6958,7 +6967,7 @@
       <c r="AH131" s="21"/>
       <c r="AI131" s="21"/>
     </row>
-    <row r="132" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A132" s="21"/>
       <c r="B132" s="44"/>
       <c r="C132" s="44"/>
@@ -6995,7 +7004,7 @@
       <c r="AH132" s="21"/>
       <c r="AI132" s="21"/>
     </row>
-    <row r="133" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A133" s="21"/>
       <c r="B133" s="44"/>
       <c r="C133" s="44"/>
@@ -7032,7 +7041,7 @@
       <c r="AH133" s="21"/>
       <c r="AI133" s="21"/>
     </row>
-    <row r="134" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A134" s="21"/>
       <c r="B134" s="44"/>
       <c r="C134" s="44"/>
@@ -7069,7 +7078,7 @@
       <c r="AH134" s="21"/>
       <c r="AI134" s="21"/>
     </row>
-    <row r="135" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A135" s="21"/>
       <c r="B135" s="44"/>
       <c r="C135" s="44"/>
@@ -7106,7 +7115,7 @@
       <c r="AH135" s="21"/>
       <c r="AI135" s="21"/>
     </row>
-    <row r="136" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A136" s="21"/>
       <c r="B136" s="44"/>
       <c r="C136" s="44"/>
@@ -7143,7 +7152,7 @@
       <c r="AH136" s="21"/>
       <c r="AI136" s="21"/>
     </row>
-    <row r="137" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A137" s="21"/>
       <c r="B137" s="44"/>
       <c r="C137" s="44"/>
@@ -7180,7 +7189,7 @@
       <c r="AH137" s="21"/>
       <c r="AI137" s="21"/>
     </row>
-    <row r="138" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A138" s="21"/>
       <c r="B138" s="44"/>
       <c r="C138" s="44"/>
@@ -7217,7 +7226,7 @@
       <c r="AH138" s="21"/>
       <c r="AI138" s="21"/>
     </row>
-    <row r="139" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A139" s="21"/>
       <c r="B139" s="44"/>
       <c r="C139" s="44"/>
@@ -7254,7 +7263,7 @@
       <c r="AH139" s="21"/>
       <c r="AI139" s="21"/>
     </row>
-    <row r="140" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A140" s="21"/>
       <c r="B140" s="44"/>
       <c r="C140" s="44"/>
@@ -7291,7 +7300,7 @@
       <c r="AH140" s="21"/>
       <c r="AI140" s="21"/>
     </row>
-    <row r="141" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A141" s="21"/>
       <c r="B141" s="44"/>
       <c r="C141" s="44"/>
@@ -7328,7 +7337,7 @@
       <c r="AH141" s="21"/>
       <c r="AI141" s="21"/>
     </row>
-    <row r="142" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A142" s="21"/>
       <c r="B142" s="44"/>
       <c r="C142" s="44"/>
@@ -7365,7 +7374,7 @@
       <c r="AH142" s="21"/>
       <c r="AI142" s="21"/>
     </row>
-    <row r="143" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A143" s="21"/>
       <c r="B143" s="44"/>
       <c r="C143" s="44"/>
@@ -7402,7 +7411,7 @@
       <c r="AH143" s="21"/>
       <c r="AI143" s="21"/>
     </row>
-    <row r="144" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A144" s="21"/>
       <c r="B144" s="44"/>
       <c r="C144" s="44"/>
@@ -7735,22 +7744,96 @@
       <c r="AH152" s="21"/>
       <c r="AI152" s="21"/>
     </row>
+    <row r="153" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A153" s="21"/>
+      <c r="B153" s="44"/>
+      <c r="C153" s="44"/>
+      <c r="D153" s="21"/>
+      <c r="E153" s="21"/>
+      <c r="F153" s="21"/>
+      <c r="G153" s="21"/>
+      <c r="H153" s="21"/>
+      <c r="I153" s="21"/>
+      <c r="J153" s="21"/>
+      <c r="K153" s="21"/>
+      <c r="L153" s="21"/>
+      <c r="M153" s="21"/>
+      <c r="N153" s="21"/>
+      <c r="O153" s="21"/>
+      <c r="P153" s="21"/>
+      <c r="Q153" s="21"/>
+      <c r="R153" s="21"/>
+      <c r="S153" s="21"/>
+      <c r="T153" s="21"/>
+      <c r="U153" s="21"/>
+      <c r="V153" s="21"/>
+      <c r="W153" s="21"/>
+      <c r="X153" s="21"/>
+      <c r="Y153" s="21"/>
+      <c r="Z153" s="21"/>
+      <c r="AA153" s="21"/>
+      <c r="AB153" s="21"/>
+      <c r="AC153" s="21"/>
+      <c r="AD153" s="21"/>
+      <c r="AE153" s="21"/>
+      <c r="AF153" s="21"/>
+      <c r="AG153" s="21"/>
+      <c r="AH153" s="21"/>
+      <c r="AI153" s="21"/>
+    </row>
+    <row r="154" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A154" s="21"/>
+      <c r="B154" s="44"/>
+      <c r="C154" s="44"/>
+      <c r="D154" s="21"/>
+      <c r="E154" s="21"/>
+      <c r="F154" s="21"/>
+      <c r="G154" s="21"/>
+      <c r="H154" s="21"/>
+      <c r="I154" s="21"/>
+      <c r="J154" s="21"/>
+      <c r="K154" s="21"/>
+      <c r="L154" s="21"/>
+      <c r="M154" s="21"/>
+      <c r="N154" s="21"/>
+      <c r="O154" s="21"/>
+      <c r="P154" s="21"/>
+      <c r="Q154" s="21"/>
+      <c r="R154" s="21"/>
+      <c r="S154" s="21"/>
+      <c r="T154" s="21"/>
+      <c r="U154" s="21"/>
+      <c r="V154" s="21"/>
+      <c r="W154" s="21"/>
+      <c r="X154" s="21"/>
+      <c r="Y154" s="21"/>
+      <c r="Z154" s="21"/>
+      <c r="AA154" s="21"/>
+      <c r="AB154" s="21"/>
+      <c r="AC154" s="21"/>
+      <c r="AD154" s="21"/>
+      <c r="AE154" s="21"/>
+      <c r="AF154" s="21"/>
+      <c r="AG154" s="21"/>
+      <c r="AH154" s="21"/>
+      <c r="AI154" s="21"/>
+    </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A116:AJ116"/>
-    <mergeCell ref="A126:AJ126"/>
+    <mergeCell ref="A118:AJ118"/>
+    <mergeCell ref="A128:AJ128"/>
     <mergeCell ref="C6:C8"/>
     <mergeCell ref="C10:C14"/>
-    <mergeCell ref="C107:C111"/>
-    <mergeCell ref="B1:B111"/>
-    <mergeCell ref="A1:A111"/>
-    <mergeCell ref="C60:C73"/>
-    <mergeCell ref="C76:C105"/>
+    <mergeCell ref="C109:C113"/>
+    <mergeCell ref="B1:B113"/>
+    <mergeCell ref="A1:A113"/>
+    <mergeCell ref="C61:C74"/>
+    <mergeCell ref="C77:C107"/>
     <mergeCell ref="C15:C20"/>
     <mergeCell ref="C21:C30"/>
     <mergeCell ref="C31:C39"/>
-    <mergeCell ref="C40:C50"/>
-    <mergeCell ref="C51:C58"/>
+    <mergeCell ref="C40:C51"/>
+    <mergeCell ref="C52:C59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>